<commit_message>
modified normalization technique to standard scaler in the preprocessing file, updating the processed_responses excel file, and ran new regression in regression_analysis_results_version2
</commit_message>
<xml_diff>
--- a/items_maps/dropped_lines.xlsx
+++ b/items_maps/dropped_lines.xlsx
@@ -891,3083 +891,3083 @@
     </row>
     <row r="2" spans="1:85">
       <c r="A2">
-        <v>0.6666666666666666</v>
+        <v>-0.3088476044477176</v>
       </c>
       <c r="B2">
-        <v>0.6666666666666666</v>
+        <v>-0.4365385085865857</v>
       </c>
       <c r="C2">
-        <v>0.6666666666666666</v>
+        <v>-0.3617626333365028</v>
       </c>
       <c r="D2">
-        <v>0.6666666666666666</v>
+        <v>-0.2260313209104581</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>-0.9616777722495112</v>
       </c>
       <c r="F2">
-        <v>0.3333333333333333</v>
+        <v>-1.60286130892507</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>-1.013380123583798</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>-0.8822565151649595</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>-1.210969514755994</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>-1.38947828638376</v>
       </c>
       <c r="K2">
-        <v>0.5</v>
+        <v>-0.8938288347265028</v>
       </c>
       <c r="L2">
-        <v>0.5</v>
+        <v>-0.427810093372549</v>
       </c>
       <c r="M2">
-        <v>0.75</v>
+        <v>0.3074890092404042</v>
       </c>
       <c r="N2">
-        <v>0.5</v>
+        <v>-1.565724865724725</v>
       </c>
       <c r="O2">
-        <v>0.3333333333333333</v>
+        <v>-2.003020160612881</v>
       </c>
       <c r="P2">
-        <v>0.25</v>
+        <v>-2.711475924852187</v>
       </c>
       <c r="Q2">
-        <v>0.5</v>
+        <v>-0.08505284855852796</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>-2.142734977684925</v>
       </c>
       <c r="S2">
-        <v>0.5555555555555555</v>
+        <v>-1.194958832147968</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>-3.147220578460181</v>
       </c>
       <c r="U2">
-        <v>0.25</v>
+        <v>-2.956715338615965</v>
       </c>
       <c r="V2">
-        <v>0.4444444444444445</v>
+        <v>-1.038220083483159</v>
       </c>
       <c r="W2">
-        <v>0.25</v>
+        <v>-2.112995445365708</v>
       </c>
       <c r="X2">
-        <v>0.25</v>
+        <v>-2.704761137794541</v>
       </c>
       <c r="Y2">
-        <v>0.75</v>
+        <v>0.6837102850692039</v>
       </c>
       <c r="Z2">
-        <v>0.75</v>
+        <v>0.486199504743121</v>
       </c>
       <c r="AA2">
-        <v>0.75</v>
+        <v>0.5011273261993328</v>
       </c>
       <c r="AB2">
-        <v>0.75</v>
+        <v>0.8221775278484124</v>
       </c>
       <c r="AC2">
-        <v>0.25</v>
+        <v>-1.871582081754603</v>
       </c>
       <c r="AD2">
-        <v>0.5</v>
+        <v>-0.3675822075682514</v>
       </c>
       <c r="AE2">
-        <v>0.25</v>
+        <v>-1.929585043810508</v>
       </c>
       <c r="AF2">
-        <v>0.5</v>
+        <v>-0.8768812412626135</v>
       </c>
       <c r="AG2">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH2">
-        <v>0</v>
+        <v>-1.066714224172605</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>-0.5686640241463884</v>
       </c>
       <c r="AJ2">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK2">
-        <v>1</v>
+        <v>1.074178219906482</v>
       </c>
       <c r="AL2">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM2">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN2">
-        <v>1</v>
+        <v>5.244322210914872</v>
       </c>
       <c r="AO2">
-        <v>1</v>
+        <v>3.112943213727974</v>
       </c>
       <c r="AP2">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ2">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR2">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS2">
-        <v>1</v>
+        <v>2.362168183855273</v>
       </c>
       <c r="AT2">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="AU2">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV2">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW2">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX2">
-        <v>0.5</v>
+        <v>0.1432175903843125</v>
       </c>
       <c r="AY2">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ2">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA2">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB2">
-        <v>1</v>
+        <v>0.6860951906939206</v>
       </c>
       <c r="BC2">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD2">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE2">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF2">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG2">
-        <v>0.25</v>
+        <v>-0.937367177234963</v>
       </c>
       <c r="BH2">
-        <v>0.5</v>
+        <v>-0.6707054826559437</v>
       </c>
       <c r="BI2">
-        <v>0</v>
+        <v>-0.8409631023746879</v>
       </c>
       <c r="BJ2">
-        <v>0.5</v>
+        <v>-0.3284539783201077</v>
       </c>
       <c r="BK2">
-        <v>1</v>
+        <v>1.067172391069504</v>
       </c>
       <c r="BL2">
-        <v>0.75</v>
+        <v>0.3674182923866799</v>
       </c>
       <c r="BM2">
-        <v>0.75</v>
+        <v>0.4605627942900607</v>
       </c>
       <c r="BN2">
-        <v>0.5</v>
+        <v>-0.3053974600325877</v>
       </c>
       <c r="BO2">
-        <v>0.75</v>
+        <v>0.335586194236475</v>
       </c>
       <c r="BP2">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ2">
-        <v>0.75</v>
+        <v>0.9394641687324224</v>
       </c>
       <c r="BR2">
-        <v>0</v>
+        <v>-0.6400564601486658</v>
       </c>
       <c r="BS2">
-        <v>1</v>
+        <v>2.191260187861297</v>
       </c>
       <c r="BT2">
-        <v>1</v>
+        <v>0.9783665806745229</v>
       </c>
       <c r="BU2">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="BV2">
-        <v>0.75</v>
+        <v>0.657827488493832</v>
       </c>
       <c r="BW2">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX2">
-        <v>0</v>
+        <v>-1.053765547986848</v>
       </c>
       <c r="BY2">
-        <v>0</v>
+        <v>-0.798339141401895</v>
       </c>
       <c r="BZ2">
-        <v>0</v>
+        <v>-0.5109474341818052</v>
       </c>
       <c r="CA2">
-        <v>0</v>
+        <v>-0.6319155142804664</v>
       </c>
       <c r="CB2">
-        <v>0.75</v>
+        <v>-0.4962523746607706</v>
       </c>
       <c r="CC2">
-        <v>0</v>
+        <v>-0.7890915148059675</v>
       </c>
       <c r="CD2">
-        <v>0.1666666666666667</v>
+        <v>-0.8805148917474771</v>
       </c>
       <c r="CE2">
-        <v>0.5</v>
+        <v>0.829382348286514</v>
       </c>
       <c r="CF2">
-        <v>0</v>
+        <v>-1.086857580798712</v>
       </c>
       <c r="CG2">
-        <v>0.5</v>
+        <v>-0.07860656409769635</v>
       </c>
     </row>
     <row r="3" spans="1:85">
       <c r="A3">
-        <v>0.6666666666666666</v>
+        <v>-0.3088476044477176</v>
       </c>
       <c r="B3">
-        <v>0.6666666666666666</v>
+        <v>-0.4365385085865857</v>
       </c>
       <c r="C3">
-        <v>0.3333333333333333</v>
+        <v>-2.03369264145926</v>
       </c>
       <c r="D3">
-        <v>0.6666666666666666</v>
+        <v>-0.2260313209104581</v>
       </c>
       <c r="E3">
-        <v>0.75</v>
+        <v>0.1803145822967834</v>
       </c>
       <c r="F3">
-        <v>0.6666666666666666</v>
+        <v>-0.235245813996465</v>
       </c>
       <c r="G3">
-        <v>0.75</v>
+        <v>0.1900087731719623</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>1.342846313523137</v>
       </c>
       <c r="I3">
-        <v>0.75</v>
+        <v>0.1603933132127148</v>
       </c>
       <c r="J3">
-        <v>0.5</v>
+        <v>-1.38947828638376</v>
       </c>
       <c r="K3">
-        <v>0.5</v>
+        <v>-0.8938288347265028</v>
       </c>
       <c r="L3">
-        <v>0.75</v>
+        <v>0.6355149937780624</v>
       </c>
       <c r="M3">
-        <v>0.75</v>
+        <v>0.3074890092404042</v>
       </c>
       <c r="N3">
-        <v>0.5</v>
+        <v>-1.565724865724725</v>
       </c>
       <c r="O3">
-        <v>0.6666666666666666</v>
+        <v>-0.6289483304324449</v>
       </c>
       <c r="P3">
-        <v>0.5</v>
+        <v>-1.516056590373652</v>
       </c>
       <c r="Q3">
-        <v>0.75</v>
+        <v>0.6095454146694497</v>
       </c>
       <c r="R3">
-        <v>0.6666666666666666</v>
+        <v>0.06434639572627425</v>
       </c>
       <c r="S3">
-        <v>0.6666666666666666</v>
+        <v>-0.619297484638483</v>
       </c>
       <c r="T3">
-        <v>0.3333333333333333</v>
+        <v>-1.801214769966612</v>
       </c>
       <c r="U3">
-        <v>0.5</v>
+        <v>-1.698460548113142</v>
       </c>
       <c r="V3">
-        <v>0.6666666666666666</v>
+        <v>0.03601668464572096</v>
       </c>
       <c r="W3">
-        <v>0.5</v>
+        <v>-0.9840897790721913</v>
       </c>
       <c r="X3">
-        <v>0.25</v>
+        <v>-2.704761137794541</v>
       </c>
       <c r="Y3">
-        <v>0.5</v>
+        <v>-0.2252533884917919</v>
       </c>
       <c r="Z3">
-        <v>0.75</v>
+        <v>0.486199504743121</v>
       </c>
       <c r="AA3">
-        <v>0.75</v>
+        <v>0.5011273261993328</v>
       </c>
       <c r="AB3">
-        <v>0.75</v>
+        <v>0.8221775278484124</v>
       </c>
       <c r="AC3">
-        <v>0.75</v>
+        <v>0.3651867476594346</v>
       </c>
       <c r="AD3">
-        <v>0.75</v>
+        <v>0.7682799293318415</v>
       </c>
       <c r="AE3">
-        <v>0.75</v>
+        <v>0.198542512546419</v>
       </c>
       <c r="AF3">
-        <v>0.5</v>
+        <v>-0.8768812412626135</v>
       </c>
       <c r="AG3">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH3">
-        <v>0</v>
+        <v>-1.066714224172605</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <v>-0.5686640241463884</v>
       </c>
       <c r="AJ3">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK3">
-        <v>1</v>
+        <v>1.074178219906482</v>
       </c>
       <c r="AL3">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM3">
-        <v>0.5</v>
+        <v>0.7474121513615285</v>
       </c>
       <c r="AN3">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO3">
-        <v>1</v>
+        <v>3.112943213727974</v>
       </c>
       <c r="AP3">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ3">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR3">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS3">
-        <v>0</v>
+        <v>-0.4221056548469904</v>
       </c>
       <c r="AT3">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="AU3">
-        <v>1</v>
+        <v>1.625181012759954</v>
       </c>
       <c r="AV3">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW3">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX3">
-        <v>0.5</v>
+        <v>0.1432175903843125</v>
       </c>
       <c r="AY3">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ3">
-        <v>1</v>
+        <v>1.513729497088757</v>
       </c>
       <c r="BA3">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB3">
-        <v>0</v>
+        <v>-1.45327435846985</v>
       </c>
       <c r="BC3">
-        <v>1</v>
+        <v>2.56961387214014</v>
       </c>
       <c r="BD3">
-        <v>1</v>
+        <v>2.008065540912678</v>
       </c>
       <c r="BE3">
-        <v>0</v>
+        <v>-1.513729497088757</v>
       </c>
       <c r="BF3">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG3">
-        <v>0.75</v>
+        <v>1.227730073886871</v>
       </c>
       <c r="BH3">
-        <v>1</v>
+        <v>0.6945881704656511</v>
       </c>
       <c r="BI3">
-        <v>0.5</v>
+        <v>0.9451071398204696</v>
       </c>
       <c r="BJ3">
-        <v>0.75</v>
+        <v>0.6103769763782007</v>
       </c>
       <c r="BK3">
-        <v>0.75</v>
+        <v>0.3536438722842411</v>
       </c>
       <c r="BL3">
-        <v>1</v>
+        <v>1.322149158209643</v>
       </c>
       <c r="BM3">
-        <v>1</v>
+        <v>1.262456390439761</v>
       </c>
       <c r="BN3">
-        <v>1</v>
+        <v>1.258055208492452</v>
       </c>
       <c r="BO3">
-        <v>0.75</v>
+        <v>0.335586194236475</v>
       </c>
       <c r="BP3">
-        <v>0.25</v>
+        <v>0.4652684966005564</v>
       </c>
       <c r="BQ3">
-        <v>0.25</v>
+        <v>-1.02539076953112</v>
       </c>
       <c r="BR3">
-        <v>0.25</v>
+        <v>0.3186307268862352</v>
       </c>
       <c r="BS3">
-        <v>0.5</v>
+        <v>0.5098233994129192</v>
       </c>
       <c r="BT3">
-        <v>1</v>
+        <v>0.9783665806745229</v>
       </c>
       <c r="BU3">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="BV3">
-        <v>0.75</v>
+        <v>0.657827488493832</v>
       </c>
       <c r="BW3">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX3">
-        <v>1</v>
+        <v>1.44324020648285</v>
       </c>
       <c r="BY3">
-        <v>0.5</v>
+        <v>0.6939242128261701</v>
       </c>
       <c r="BZ3">
-        <v>0.5</v>
+        <v>1.215702515811881</v>
       </c>
       <c r="CA3">
-        <v>0.25</v>
+        <v>0.3400442229311928</v>
       </c>
       <c r="CB3">
-        <v>1</v>
+        <v>0.6940592652598194</v>
       </c>
       <c r="CC3">
-        <v>0.1666666666666667</v>
+        <v>-0.1492371659207503</v>
       </c>
       <c r="CD3">
-        <v>0.1666666666666667</v>
+        <v>-0.8805148917474771</v>
       </c>
       <c r="CE3">
-        <v>0.5</v>
+        <v>0.829382348286514</v>
       </c>
       <c r="CF3">
-        <v>0</v>
+        <v>-1.086857580798712</v>
       </c>
       <c r="CG3">
-        <v>0.5</v>
+        <v>-0.07860656409769635</v>
       </c>
     </row>
     <row r="4" spans="1:85">
       <c r="A4">
-        <v>0.3333333333333333</v>
+        <v>-1.645884069272012</v>
       </c>
       <c r="B4">
-        <v>0.6666666666666666</v>
+        <v>-0.4365385085865857</v>
       </c>
       <c r="C4">
-        <v>0.3333333333333333</v>
+        <v>-2.03369264145926</v>
       </c>
       <c r="D4">
-        <v>0.6666666666666666</v>
+        <v>-0.2260313209104581</v>
       </c>
       <c r="E4">
-        <v>0.25</v>
+        <v>-2.103670126795806</v>
       </c>
       <c r="F4">
-        <v>0.6666666666666666</v>
+        <v>-0.235245813996465</v>
       </c>
       <c r="G4">
-        <v>0.75</v>
+        <v>0.1900087731719623</v>
       </c>
       <c r="H4">
-        <v>0.25</v>
+        <v>-1.994807929509008</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>-1.210969514755994</v>
       </c>
       <c r="J4">
-        <v>0.75</v>
+        <v>-0.2044369548544679</v>
       </c>
       <c r="K4">
-        <v>0.75</v>
+        <v>0.159721991085148</v>
       </c>
       <c r="L4">
-        <v>0.5</v>
+        <v>-0.427810093372549</v>
       </c>
       <c r="M4">
-        <v>0.6666666666666666</v>
+        <v>-0.1160801882273011</v>
       </c>
       <c r="N4">
-        <v>0.5</v>
+        <v>-1.565724865724725</v>
       </c>
       <c r="O4">
-        <v>0.6666666666666666</v>
+        <v>-0.6289483304324449</v>
       </c>
       <c r="P4">
-        <v>0.75</v>
+        <v>-0.3206372558951174</v>
       </c>
       <c r="Q4">
-        <v>0.5</v>
+        <v>-0.08505284855852796</v>
       </c>
       <c r="R4">
-        <v>0.6666666666666666</v>
+        <v>0.06434639572627425</v>
       </c>
       <c r="S4">
-        <v>0.5555555555555555</v>
+        <v>-1.194958832147968</v>
       </c>
       <c r="T4">
-        <v>0.6666666666666666</v>
+        <v>-0.4552089614730434</v>
       </c>
       <c r="U4">
-        <v>0.75</v>
+        <v>-0.4402057576103177</v>
       </c>
       <c r="V4">
-        <v>0.6666666666666666</v>
+        <v>0.03601668464572096</v>
       </c>
       <c r="W4">
-        <v>0.75</v>
+        <v>0.1448158872213257</v>
       </c>
       <c r="X4">
-        <v>0.5</v>
+        <v>-1.452759693444301</v>
       </c>
       <c r="Y4">
-        <v>0.5</v>
+        <v>-0.2252533884917919</v>
       </c>
       <c r="Z4">
-        <v>0.5</v>
+        <v>-0.4506905521495219</v>
       </c>
       <c r="AA4">
-        <v>0.5</v>
+        <v>-0.4433049424071018</v>
       </c>
       <c r="AB4">
-        <v>0.5</v>
+        <v>-0.1708044864192125</v>
       </c>
       <c r="AC4">
-        <v>0.75</v>
+        <v>0.3651867476594346</v>
       </c>
       <c r="AD4">
-        <v>0.5</v>
+        <v>-0.3675822075682514</v>
       </c>
       <c r="AE4">
-        <v>0.75</v>
+        <v>0.198542512546419</v>
       </c>
       <c r="AF4">
-        <v>0.5</v>
+        <v>-0.8768812412626135</v>
       </c>
       <c r="AG4">
-        <v>1</v>
+        <v>2.168620633466131</v>
       </c>
       <c r="AH4">
-        <v>0.3333333333333333</v>
+        <v>-0.04754158102162029</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>-0.5686640241463884</v>
       </c>
       <c r="AJ4">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK4">
-        <v>1</v>
+        <v>1.074178219906482</v>
       </c>
       <c r="AL4">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM4">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN4">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO4">
-        <v>0</v>
+        <v>-0.32030283871156</v>
       </c>
       <c r="AP4">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ4">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR4">
-        <v>1</v>
+        <v>6.083002174247108</v>
       </c>
       <c r="AS4">
-        <v>0</v>
+        <v>-0.4221056548469904</v>
       </c>
       <c r="AT4">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="AU4">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV4">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW4">
-        <v>1</v>
+        <v>2.065055426237636</v>
       </c>
       <c r="AX4">
-        <v>0</v>
+        <v>-1.217349518266656</v>
       </c>
       <c r="AY4">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ4">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA4">
-        <v>1</v>
+        <v>2.065055426237636</v>
       </c>
       <c r="BB4">
-        <v>0</v>
+        <v>-1.45327435846985</v>
       </c>
       <c r="BC4">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD4">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE4">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF4">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG4">
-        <v>0.5</v>
+        <v>0.145181448325954</v>
       </c>
       <c r="BH4">
-        <v>0.25</v>
+        <v>-1.353352309216741</v>
       </c>
       <c r="BI4">
-        <v>0</v>
+        <v>-0.8409631023746879</v>
       </c>
       <c r="BJ4">
-        <v>0.5</v>
+        <v>-0.3284539783201077</v>
       </c>
       <c r="BK4">
-        <v>0</v>
+        <v>-1.786941684071548</v>
       </c>
       <c r="BL4">
-        <v>1</v>
+        <v>1.322149158209643</v>
       </c>
       <c r="BM4">
-        <v>0.75</v>
+        <v>0.4605627942900607</v>
       </c>
       <c r="BN4">
-        <v>0</v>
+        <v>-1.868850128557627</v>
       </c>
       <c r="BO4">
-        <v>0.75</v>
+        <v>0.335586194236475</v>
       </c>
       <c r="BP4">
-        <v>0.75</v>
+        <v>2.621850852465298</v>
       </c>
       <c r="BQ4">
-        <v>0.75</v>
+        <v>0.9394641687324224</v>
       </c>
       <c r="BR4">
-        <v>0.5</v>
+        <v>1.277317913921136</v>
       </c>
       <c r="BS4">
-        <v>0</v>
+        <v>-1.171613389035458</v>
       </c>
       <c r="BT4">
-        <v>1</v>
+        <v>0.9783665806745229</v>
       </c>
       <c r="BU4">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="BV4">
-        <v>0</v>
+        <v>-1.55427867379425</v>
       </c>
       <c r="BW4">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX4">
-        <v>0</v>
+        <v>-1.053765547986848</v>
       </c>
       <c r="BY4">
-        <v>0</v>
+        <v>-0.798339141401895</v>
       </c>
       <c r="BZ4">
-        <v>0</v>
+        <v>-0.5109474341818052</v>
       </c>
       <c r="CA4">
-        <v>0</v>
+        <v>-0.6319155142804664</v>
       </c>
       <c r="CB4">
-        <v>1</v>
+        <v>0.6940592652598194</v>
       </c>
       <c r="CC4">
-        <v>0.1666666666666667</v>
+        <v>-0.1492371659207503</v>
       </c>
       <c r="CD4">
-        <v>0.6666666666666666</v>
+        <v>0.6048126879380211</v>
       </c>
       <c r="CE4">
-        <v>0.5</v>
+        <v>0.829382348286514</v>
       </c>
       <c r="CF4">
-        <v>1</v>
+        <v>0.9174012913193432</v>
       </c>
       <c r="CG4">
-        <v>0.5</v>
+        <v>-0.07860656409769635</v>
       </c>
     </row>
     <row r="5" spans="1:85">
       <c r="A5">
-        <v>1</v>
+        <v>1.028188860376577</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>1.154714764648387</v>
       </c>
       <c r="C5">
-        <v>0.6666666666666666</v>
+        <v>-0.3617626333365028</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>1.228245668343623</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>-0.9616777722495112</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>1.13236968093214</v>
       </c>
       <c r="G5">
-        <v>0.75</v>
+        <v>0.1900087731719623</v>
       </c>
       <c r="H5">
-        <v>0.75</v>
+        <v>0.2302948991790885</v>
       </c>
       <c r="I5">
-        <v>0.75</v>
+        <v>0.1603933132127148</v>
       </c>
       <c r="J5">
-        <v>0.75</v>
+        <v>-0.2044369548544679</v>
       </c>
       <c r="K5">
-        <v>0.5</v>
+        <v>-0.8938288347265028</v>
       </c>
       <c r="L5">
-        <v>0.5</v>
+        <v>-0.427810093372549</v>
       </c>
       <c r="M5">
-        <v>0.75</v>
+        <v>0.3074890092404042</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0.8753825385642784</v>
       </c>
       <c r="O5">
-        <v>0.3333333333333333</v>
+        <v>-2.003020160612881</v>
       </c>
       <c r="P5">
-        <v>0.75</v>
+        <v>-0.3206372558951174</v>
       </c>
       <c r="Q5">
-        <v>0.5</v>
+        <v>-0.08505284855852796</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>-2.142734977684925</v>
       </c>
       <c r="S5">
-        <v>0.6666666666666666</v>
+        <v>-0.619297484638483</v>
       </c>
       <c r="T5">
-        <v>0.6666666666666666</v>
+        <v>-0.4552089614730434</v>
       </c>
       <c r="U5">
-        <v>0.75</v>
+        <v>-0.4402057576103177</v>
       </c>
       <c r="V5">
-        <v>0.6666666666666666</v>
+        <v>0.03601668464572096</v>
       </c>
       <c r="W5">
-        <v>0.75</v>
+        <v>0.1448158872213257</v>
       </c>
       <c r="X5">
-        <v>0.75</v>
+        <v>-0.2007582490940618</v>
       </c>
       <c r="Y5">
-        <v>0.25</v>
+        <v>-1.134217062052788</v>
       </c>
       <c r="Z5">
-        <v>0.5</v>
+        <v>-0.4506905521495219</v>
       </c>
       <c r="AA5">
-        <v>1</v>
+        <v>1.445559594805767</v>
       </c>
       <c r="AB5">
-        <v>0.25</v>
+        <v>-1.163786500686837</v>
       </c>
       <c r="AC5">
-        <v>0.75</v>
+        <v>0.3651867476594346</v>
       </c>
       <c r="AD5">
-        <v>0.75</v>
+        <v>0.7682799293318415</v>
       </c>
       <c r="AE5">
-        <v>1</v>
+        <v>1.262606290724883</v>
       </c>
       <c r="AF5">
-        <v>1</v>
+        <v>1.491388567816728</v>
       </c>
       <c r="AG5">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH5">
-        <v>0</v>
+        <v>-1.066714224172605</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>-0.5686640241463884</v>
       </c>
       <c r="AJ5">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK5">
-        <v>0</v>
+        <v>-0.9282300922017971</v>
       </c>
       <c r="AL5">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM5">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN5">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO5">
-        <v>0</v>
+        <v>-0.32030283871156</v>
       </c>
       <c r="AP5">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ5">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR5">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS5">
-        <v>1</v>
+        <v>2.362168183855273</v>
       </c>
       <c r="AT5">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="AU5">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV5">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW5">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX5">
-        <v>0</v>
+        <v>-1.217349518266656</v>
       </c>
       <c r="AY5">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ5">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA5">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB5">
-        <v>0</v>
+        <v>-1.45327435846985</v>
       </c>
       <c r="BC5">
-        <v>1</v>
+        <v>2.56961387214014</v>
       </c>
       <c r="BD5">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE5">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF5">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG5">
-        <v>0.25</v>
+        <v>-0.937367177234963</v>
       </c>
       <c r="BH5">
-        <v>1</v>
+        <v>0.6945881704656511</v>
       </c>
       <c r="BI5">
-        <v>0.25</v>
+        <v>0.05207201872289086</v>
       </c>
       <c r="BJ5">
-        <v>0.5</v>
+        <v>-0.3284539783201077</v>
       </c>
       <c r="BK5">
-        <v>0.75</v>
+        <v>0.3536438722842411</v>
       </c>
       <c r="BL5">
-        <v>1</v>
+        <v>1.322149158209643</v>
       </c>
       <c r="BM5">
-        <v>0.75</v>
+        <v>0.4605627942900607</v>
       </c>
       <c r="BN5">
-        <v>0.75</v>
+        <v>0.4763288742299319</v>
       </c>
       <c r="BO5">
-        <v>0.25</v>
+        <v>-1.421758303826287</v>
       </c>
       <c r="BP5">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ5">
-        <v>0.75</v>
+        <v>0.9394641687324224</v>
       </c>
       <c r="BR5">
-        <v>0.25</v>
+        <v>0.3186307268862352</v>
       </c>
       <c r="BS5">
-        <v>0.5</v>
+        <v>0.5098233994129192</v>
       </c>
       <c r="BT5">
-        <v>1</v>
+        <v>0.9783665806745229</v>
       </c>
       <c r="BU5">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="BV5">
-        <v>0.5</v>
+        <v>-0.07954123226886212</v>
       </c>
       <c r="BW5">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX5">
-        <v>1</v>
+        <v>1.44324020648285</v>
       </c>
       <c r="BY5">
-        <v>0</v>
+        <v>-0.798339141401895</v>
       </c>
       <c r="BZ5">
-        <v>0</v>
+        <v>-0.5109474341818052</v>
       </c>
       <c r="CA5">
-        <v>0</v>
+        <v>-0.6319155142804664</v>
       </c>
       <c r="CB5">
-        <v>1</v>
+        <v>0.6940592652598194</v>
       </c>
       <c r="CC5">
-        <v>0</v>
+        <v>-0.7890915148059675</v>
       </c>
       <c r="CD5">
-        <v>0.1666666666666667</v>
+        <v>-0.8805148917474771</v>
       </c>
       <c r="CE5">
-        <v>0</v>
+        <v>-1.173984873278798</v>
       </c>
       <c r="CF5">
-        <v>0</v>
+        <v>-1.086857580798712</v>
       </c>
       <c r="CG5">
-        <v>0.25</v>
+        <v>-1.115608544309615</v>
       </c>
     </row>
     <row r="6" spans="1:85">
       <c r="B6">
-        <v>1</v>
+        <v>1.154714764648387</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>1.310167374786254</v>
       </c>
       <c r="D6">
-        <v>0.6666666666666666</v>
+        <v>-0.2260313209104581</v>
       </c>
       <c r="E6">
-        <v>0.75</v>
+        <v>0.1803145822967834</v>
       </c>
       <c r="F6">
-        <v>0.6666666666666666</v>
+        <v>-0.235245813996465</v>
       </c>
       <c r="G6">
-        <v>0.75</v>
+        <v>0.1900087731719623</v>
       </c>
       <c r="H6">
-        <v>0.75</v>
+        <v>0.2302948991790885</v>
       </c>
       <c r="I6">
-        <v>0.75</v>
+        <v>0.1603933132127148</v>
       </c>
       <c r="J6">
-        <v>0.75</v>
+        <v>-0.2044369548544679</v>
       </c>
       <c r="K6">
-        <v>0.5</v>
+        <v>-0.8938288347265028</v>
       </c>
       <c r="L6">
-        <v>0.25</v>
+        <v>-1.49113518052316</v>
       </c>
       <c r="M6">
-        <v>0.6666666666666666</v>
+        <v>-0.1160801882273011</v>
       </c>
       <c r="N6">
-        <v>0.5</v>
+        <v>-1.565724865724725</v>
       </c>
       <c r="O6">
-        <v>0.6666666666666666</v>
+        <v>-0.6289483304324449</v>
       </c>
       <c r="P6">
-        <v>0.75</v>
+        <v>-0.3206372558951174</v>
       </c>
       <c r="Q6">
-        <v>0.75</v>
+        <v>0.6095454146694497</v>
       </c>
       <c r="R6">
-        <v>0.6666666666666666</v>
+        <v>0.06434639572627425</v>
       </c>
       <c r="S6">
-        <v>0.6666666666666666</v>
+        <v>-0.619297484638483</v>
       </c>
       <c r="T6">
-        <v>0.6666666666666666</v>
+        <v>-0.4552089614730434</v>
       </c>
       <c r="U6">
-        <v>0.75</v>
+        <v>-0.4402057576103177</v>
       </c>
       <c r="V6">
-        <v>0.6666666666666666</v>
+        <v>0.03601668464572096</v>
       </c>
       <c r="W6">
-        <v>0.75</v>
+        <v>0.1448158872213257</v>
       </c>
       <c r="X6">
-        <v>0.75</v>
+        <v>-0.2007582490940618</v>
       </c>
       <c r="Y6">
-        <v>0.25</v>
+        <v>-1.134217062052788</v>
       </c>
       <c r="Z6">
-        <v>0.5</v>
+        <v>-0.4506905521495219</v>
       </c>
       <c r="AA6">
-        <v>0.5</v>
+        <v>-0.4433049424071018</v>
       </c>
       <c r="AB6">
-        <v>0.5</v>
+        <v>-0.1708044864192125</v>
       </c>
       <c r="AC6">
-        <v>0.5</v>
+        <v>-0.7531976670475842</v>
       </c>
       <c r="AD6">
-        <v>0.75</v>
+        <v>0.7682799293318415</v>
       </c>
       <c r="AE6">
-        <v>0.75</v>
+        <v>0.198542512546419</v>
       </c>
       <c r="AF6">
-        <v>0.75</v>
+        <v>0.3072536632770573</v>
       </c>
       <c r="AG6">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH6">
-        <v>0.6666666666666666</v>
+        <v>0.9716310621293642</v>
       </c>
       <c r="AI6">
-        <v>1</v>
+        <v>1.753380741118031</v>
       </c>
       <c r="AJ6">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK6">
-        <v>0</v>
+        <v>-0.9282300922017971</v>
       </c>
       <c r="AL6">
-        <v>0.6666666666666666</v>
+        <v>1.713392545761488</v>
       </c>
       <c r="AM6">
-        <v>0.5</v>
+        <v>0.7474121513615285</v>
       </c>
       <c r="AN6">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO6">
-        <v>0</v>
+        <v>-0.32030283871156</v>
       </c>
       <c r="AP6">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ6">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR6">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS6">
-        <v>0</v>
+        <v>-0.4221056548469904</v>
       </c>
       <c r="AT6">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="AU6">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV6">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW6">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX6">
-        <v>0.5</v>
+        <v>0.1432175903843125</v>
       </c>
       <c r="AY6">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ6">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA6">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB6">
-        <v>1</v>
+        <v>0.6860951906939206</v>
       </c>
       <c r="BC6">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD6">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE6">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF6">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG6">
-        <v>0.25</v>
+        <v>-0.937367177234963</v>
       </c>
       <c r="BH6">
-        <v>0.75</v>
+        <v>0.0119413439048537</v>
       </c>
       <c r="BI6">
-        <v>0.5</v>
+        <v>0.9451071398204696</v>
       </c>
       <c r="BJ6">
-        <v>0.5</v>
+        <v>-0.3284539783201077</v>
       </c>
       <c r="BK6">
-        <v>0.75</v>
+        <v>0.3536438722842411</v>
       </c>
       <c r="BL6">
-        <v>0.75</v>
+        <v>0.3674182923866799</v>
       </c>
       <c r="BM6">
-        <v>0</v>
+        <v>-1.945117994159039</v>
       </c>
       <c r="BN6">
-        <v>0.5</v>
+        <v>-0.3053974600325877</v>
       </c>
       <c r="BO6">
-        <v>0.5</v>
+        <v>-0.543086054794906</v>
       </c>
       <c r="BP6">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ6">
-        <v>0.5</v>
+        <v>-0.04296330039934874</v>
       </c>
       <c r="BR6">
-        <v>0.5</v>
+        <v>1.277317913921136</v>
       </c>
       <c r="BS6">
-        <v>0.5</v>
+        <v>0.5098233994129192</v>
       </c>
       <c r="BT6">
-        <v>1</v>
+        <v>0.9783665806745229</v>
       </c>
       <c r="BU6">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="BV6">
-        <v>0</v>
+        <v>-1.55427867379425</v>
       </c>
       <c r="BW6">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX6">
-        <v>0</v>
+        <v>-1.053765547986848</v>
       </c>
       <c r="BY6">
-        <v>0</v>
+        <v>-0.798339141401895</v>
       </c>
       <c r="BZ6">
-        <v>0</v>
+        <v>-0.5109474341818052</v>
       </c>
       <c r="CA6">
-        <v>0</v>
+        <v>-0.6319155142804664</v>
       </c>
       <c r="CB6">
-        <v>0.5</v>
+        <v>-1.686564014581361</v>
       </c>
       <c r="CC6">
-        <v>0</v>
+        <v>-0.7890915148059675</v>
       </c>
       <c r="CD6">
-        <v>1</v>
+        <v>1.59503107439502</v>
       </c>
       <c r="CE6">
-        <v>0.5</v>
+        <v>0.829382348286514</v>
       </c>
       <c r="CF6">
-        <v>1</v>
+        <v>0.9174012913193432</v>
       </c>
       <c r="CG6">
-        <v>1</v>
+        <v>1.995397396326141</v>
       </c>
     </row>
     <row r="7" spans="1:85">
       <c r="A7">
-        <v>1</v>
+        <v>1.028188860376577</v>
       </c>
       <c r="B7">
-        <v>0.6666666666666666</v>
+        <v>-0.4365385085865857</v>
       </c>
       <c r="C7">
-        <v>0.6666666666666666</v>
+        <v>-0.3617626333365028</v>
       </c>
       <c r="D7">
-        <v>0.6666666666666666</v>
+        <v>-0.2260313209104581</v>
       </c>
       <c r="E7">
-        <v>0.75</v>
+        <v>0.1803145822967834</v>
       </c>
       <c r="F7">
-        <v>0.6666666666666666</v>
+        <v>-0.235245813996465</v>
       </c>
       <c r="G7">
-        <v>0.75</v>
+        <v>0.1900087731719623</v>
       </c>
       <c r="H7">
-        <v>0.75</v>
+        <v>0.2302948991790885</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>-1.210969514755994</v>
       </c>
       <c r="J7">
-        <v>0.75</v>
+        <v>-0.2044369548544679</v>
       </c>
       <c r="K7">
-        <v>0.5</v>
+        <v>-0.8938288347265028</v>
       </c>
       <c r="L7">
-        <v>0.5</v>
+        <v>-0.427810093372549</v>
       </c>
       <c r="M7">
-        <v>0.75</v>
+        <v>0.3074890092404042</v>
       </c>
       <c r="N7">
-        <v>0.75</v>
+        <v>-0.3451711635802232</v>
       </c>
       <c r="O7">
-        <v>0.3333333333333333</v>
+        <v>-2.003020160612881</v>
       </c>
       <c r="P7">
-        <v>0.75</v>
+        <v>-0.3206372558951174</v>
       </c>
       <c r="Q7">
-        <v>0.75</v>
+        <v>0.6095454146694497</v>
       </c>
       <c r="R7">
-        <v>0.6666666666666666</v>
+        <v>0.06434639572627425</v>
       </c>
       <c r="S7">
-        <v>0.4444444444444445</v>
+        <v>-1.770620179657452</v>
       </c>
       <c r="T7">
-        <v>0.6666666666666666</v>
+        <v>-0.4552089614730434</v>
       </c>
       <c r="U7">
-        <v>0.75</v>
+        <v>-0.4402057576103177</v>
       </c>
       <c r="V7">
-        <v>0.5555555555555555</v>
+        <v>-0.5011016994187191</v>
       </c>
       <c r="W7">
-        <v>0.75</v>
+        <v>0.1448158872213257</v>
       </c>
       <c r="X7">
-        <v>0.75</v>
+        <v>-0.2007582490940618</v>
       </c>
       <c r="Y7">
-        <v>0.5</v>
+        <v>-0.2252533884917919</v>
       </c>
       <c r="Z7">
-        <v>0.5</v>
+        <v>-0.4506905521495219</v>
       </c>
       <c r="AA7">
-        <v>0.5</v>
+        <v>-0.4433049424071018</v>
       </c>
       <c r="AB7">
-        <v>0.5</v>
+        <v>-0.1708044864192125</v>
       </c>
       <c r="AC7">
-        <v>0.75</v>
+        <v>0.3651867476594346</v>
       </c>
       <c r="AD7">
-        <v>0.5</v>
+        <v>-0.3675822075682514</v>
       </c>
       <c r="AE7">
-        <v>0.5</v>
+        <v>-0.8655212656320448</v>
       </c>
       <c r="AF7">
-        <v>0.5</v>
+        <v>-0.8768812412626135</v>
       </c>
       <c r="AG7">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH7">
-        <v>0.3333333333333333</v>
+        <v>-0.04754158102162029</v>
       </c>
       <c r="AI7">
-        <v>1</v>
+        <v>1.753380741118031</v>
       </c>
       <c r="AJ7">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK7">
-        <v>0</v>
+        <v>-0.9282300922017971</v>
       </c>
       <c r="AL7">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM7">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN7">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO7">
-        <v>0</v>
+        <v>-0.32030283871156</v>
       </c>
       <c r="AP7">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ7">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR7">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS7">
-        <v>0</v>
+        <v>-0.4221056548469904</v>
       </c>
       <c r="AT7">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="AU7">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV7">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW7">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX7">
-        <v>0</v>
+        <v>-1.217349518266656</v>
       </c>
       <c r="AY7">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ7">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA7">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB7">
-        <v>1</v>
+        <v>0.6860951906939206</v>
       </c>
       <c r="BC7">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD7">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE7">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF7">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG7">
-        <v>0.75</v>
+        <v>1.227730073886871</v>
       </c>
       <c r="BH7">
-        <v>1</v>
+        <v>0.6945881704656511</v>
       </c>
       <c r="BI7">
-        <v>0.5</v>
+        <v>0.9451071398204696</v>
       </c>
       <c r="BJ7">
-        <v>1</v>
+        <v>1.549207931076509</v>
       </c>
       <c r="BK7">
-        <v>1</v>
+        <v>1.067172391069504</v>
       </c>
       <c r="BL7">
-        <v>1</v>
+        <v>1.322149158209643</v>
       </c>
       <c r="BM7">
-        <v>0.75</v>
+        <v>0.4605627942900607</v>
       </c>
       <c r="BN7">
-        <v>0.75</v>
+        <v>0.4763288742299319</v>
       </c>
       <c r="BO7">
-        <v>0.75</v>
+        <v>0.335586194236475</v>
       </c>
       <c r="BP7">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ7">
-        <v>0.25</v>
+        <v>-1.02539076953112</v>
       </c>
       <c r="BR7">
-        <v>0</v>
+        <v>-0.6400564601486658</v>
       </c>
       <c r="BS7">
-        <v>0.75</v>
+        <v>1.350541793637108</v>
       </c>
       <c r="BT7">
-        <v>0</v>
+        <v>-1.019131854869295</v>
       </c>
       <c r="BU7">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="BV7">
-        <v>0.75</v>
+        <v>0.657827488493832</v>
       </c>
       <c r="BW7">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX7">
-        <v>0.5</v>
+        <v>0.1947373292480012</v>
       </c>
       <c r="BY7">
-        <v>0</v>
+        <v>-0.798339141401895</v>
       </c>
       <c r="BZ7">
-        <v>0</v>
+        <v>-0.5109474341818052</v>
       </c>
       <c r="CA7">
-        <v>0</v>
+        <v>-0.6319155142804664</v>
       </c>
       <c r="CB7">
-        <v>0.75</v>
+        <v>-0.4962523746607706</v>
       </c>
       <c r="CC7">
-        <v>0</v>
+        <v>-0.7890915148059675</v>
       </c>
       <c r="CD7">
-        <v>0.8333333333333334</v>
+        <v>1.099921881166521</v>
       </c>
       <c r="CE7">
-        <v>0.5</v>
+        <v>0.829382348286514</v>
       </c>
       <c r="CF7">
-        <v>1</v>
+        <v>0.9174012913193432</v>
       </c>
       <c r="CG7">
-        <v>0.75</v>
+        <v>0.9583954161142225</v>
       </c>
     </row>
     <row r="8" spans="1:85">
       <c r="A8">
-        <v>0.3333333333333333</v>
+        <v>-1.645884069272012</v>
       </c>
       <c r="B8">
-        <v>0.6666666666666666</v>
+        <v>-0.4365385085865857</v>
       </c>
       <c r="C8">
-        <v>0.6666666666666666</v>
+        <v>-0.3617626333365028</v>
       </c>
       <c r="D8">
-        <v>0.3333333333333333</v>
+        <v>-1.680308310164539</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>-0.9616777722495112</v>
       </c>
       <c r="F8">
-        <v>0.3333333333333333</v>
+        <v>-1.60286130892507</v>
       </c>
       <c r="G8">
-        <v>0.5</v>
+        <v>-1.013380123583798</v>
       </c>
       <c r="H8">
-        <v>0.5</v>
+        <v>-0.8822565151649595</v>
       </c>
       <c r="I8">
-        <v>0.5</v>
+        <v>-1.210969514755994</v>
       </c>
       <c r="J8">
-        <v>0.5</v>
+        <v>-1.38947828638376</v>
       </c>
       <c r="K8">
-        <v>0.5</v>
+        <v>-0.8938288347265028</v>
       </c>
       <c r="L8">
-        <v>0.25</v>
+        <v>-1.49113518052316</v>
       </c>
       <c r="M8">
-        <v>0.6666666666666666</v>
+        <v>-0.1160801882273011</v>
       </c>
       <c r="N8">
-        <v>0.5</v>
+        <v>-1.565724865724725</v>
       </c>
       <c r="O8">
-        <v>0.3333333333333333</v>
+        <v>-2.003020160612881</v>
       </c>
       <c r="P8">
-        <v>0.75</v>
+        <v>-0.3206372558951174</v>
       </c>
       <c r="Q8">
-        <v>0.75</v>
+        <v>0.6095454146694497</v>
       </c>
       <c r="R8">
-        <v>0.3333333333333333</v>
+        <v>-1.039194290979325</v>
       </c>
       <c r="S8">
-        <v>0.5555555555555555</v>
+        <v>-1.194958832147968</v>
       </c>
       <c r="T8">
-        <v>0.3333333333333333</v>
+        <v>-1.801214769966612</v>
       </c>
       <c r="U8">
-        <v>0.5</v>
+        <v>-1.698460548113142</v>
       </c>
       <c r="V8">
-        <v>0.6666666666666666</v>
+        <v>0.03601668464572096</v>
       </c>
       <c r="W8">
-        <v>0.5</v>
+        <v>-0.9840897790721913</v>
       </c>
       <c r="X8">
-        <v>0.5</v>
+        <v>-1.452759693444301</v>
       </c>
       <c r="Y8">
-        <v>0.5</v>
+        <v>-0.2252533884917919</v>
       </c>
       <c r="Z8">
-        <v>0.25</v>
+        <v>-1.387580609042165</v>
       </c>
       <c r="AA8">
-        <v>0.25</v>
+        <v>-1.387737211013536</v>
       </c>
       <c r="AB8">
-        <v>0.25</v>
+        <v>-1.163786500686837</v>
       </c>
       <c r="AC8">
-        <v>0.5</v>
+        <v>-0.7531976670475842</v>
       </c>
       <c r="AD8">
-        <v>0.5</v>
+        <v>-0.3675822075682514</v>
       </c>
       <c r="AE8">
-        <v>0.5</v>
+        <v>-0.8655212656320448</v>
       </c>
       <c r="AF8">
-        <v>0.5</v>
+        <v>-0.8768812412626135</v>
       </c>
       <c r="AG8">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH8">
-        <v>0.6666666666666666</v>
+        <v>0.9716310621293642</v>
       </c>
       <c r="AI8">
-        <v>0</v>
+        <v>-0.5686640241463884</v>
       </c>
       <c r="AJ8">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK8">
-        <v>0</v>
+        <v>-0.9282300922017971</v>
       </c>
       <c r="AL8">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM8">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN8">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO8">
-        <v>0</v>
+        <v>-0.32030283871156</v>
       </c>
       <c r="AP8">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ8">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR8">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS8">
-        <v>1</v>
+        <v>2.362168183855273</v>
       </c>
       <c r="AT8">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="AU8">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV8">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW8">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX8">
-        <v>1</v>
+        <v>1.503784699035281</v>
       </c>
       <c r="AY8">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ8">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA8">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB8">
-        <v>1</v>
+        <v>0.6860951906939206</v>
       </c>
       <c r="BC8">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD8">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE8">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF8">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG8">
-        <v>0.25</v>
+        <v>-0.937367177234963</v>
       </c>
       <c r="BH8">
-        <v>1</v>
+        <v>0.6945881704656511</v>
       </c>
       <c r="BI8">
-        <v>0</v>
+        <v>-0.8409631023746879</v>
       </c>
       <c r="BJ8">
-        <v>0</v>
+        <v>-2.206115887716724</v>
       </c>
       <c r="BK8">
-        <v>0.75</v>
+        <v>0.3536438722842411</v>
       </c>
       <c r="BL8">
-        <v>0.75</v>
+        <v>0.3674182923866799</v>
       </c>
       <c r="BM8">
-        <v>0.5</v>
+        <v>-0.3413308018596391</v>
       </c>
       <c r="BN8">
-        <v>0.75</v>
+        <v>0.4763288742299319</v>
       </c>
       <c r="BO8">
-        <v>0.5</v>
+        <v>-0.543086054794906</v>
       </c>
       <c r="BP8">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ8">
-        <v>0.5</v>
+        <v>-0.04296330039934874</v>
       </c>
       <c r="BR8">
-        <v>0.75</v>
+        <v>2.236005100956037</v>
       </c>
       <c r="BS8">
-        <v>0.75</v>
+        <v>1.350541793637108</v>
       </c>
       <c r="BT8">
-        <v>1</v>
+        <v>0.9783665806745229</v>
       </c>
       <c r="BU8">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="BV8">
-        <v>0.75</v>
+        <v>0.657827488493832</v>
       </c>
       <c r="BW8">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX8">
-        <v>0</v>
+        <v>-1.053765547986848</v>
       </c>
       <c r="BY8">
-        <v>0</v>
+        <v>-0.798339141401895</v>
       </c>
       <c r="BZ8">
-        <v>0</v>
+        <v>-0.5109474341818052</v>
       </c>
       <c r="CA8">
-        <v>0</v>
+        <v>-0.6319155142804664</v>
       </c>
       <c r="CB8">
-        <v>0.75</v>
+        <v>-0.4962523746607706</v>
       </c>
       <c r="CC8">
-        <v>0.8333333333333334</v>
+        <v>2.410180229620118</v>
       </c>
       <c r="CD8">
-        <v>1</v>
+        <v>1.59503107439502</v>
       </c>
       <c r="CE8">
-        <v>0.5</v>
+        <v>0.829382348286514</v>
       </c>
       <c r="CF8">
-        <v>1</v>
+        <v>0.9174012913193432</v>
       </c>
       <c r="CG8">
-        <v>0.5</v>
+        <v>-0.07860656409769635</v>
       </c>
     </row>
     <row r="9" spans="1:85">
       <c r="A9">
-        <v>0.6666666666666666</v>
+        <v>-0.3088476044477176</v>
       </c>
       <c r="B9">
-        <v>0.6666666666666666</v>
+        <v>-0.4365385085865857</v>
       </c>
       <c r="C9">
-        <v>0.6666666666666666</v>
+        <v>-0.3617626333365028</v>
       </c>
       <c r="D9">
-        <v>0.6666666666666666</v>
+        <v>-0.2260313209104581</v>
       </c>
       <c r="E9">
-        <v>0.75</v>
+        <v>0.1803145822967834</v>
       </c>
       <c r="F9">
-        <v>0.6666666666666666</v>
+        <v>-0.235245813996465</v>
       </c>
       <c r="G9">
-        <v>0.5</v>
+        <v>-1.013380123583798</v>
       </c>
       <c r="H9">
-        <v>0.25</v>
+        <v>-1.994807929509008</v>
       </c>
       <c r="I9">
-        <v>0.75</v>
+        <v>0.1603933132127148</v>
       </c>
       <c r="J9">
-        <v>0.75</v>
+        <v>-0.2044369548544679</v>
       </c>
       <c r="K9">
-        <v>0.5</v>
+        <v>-0.8938288347265028</v>
       </c>
       <c r="L9">
-        <v>0.5</v>
+        <v>-0.427810093372549</v>
       </c>
       <c r="M9">
-        <v>0.6666666666666666</v>
+        <v>-0.1160801882273011</v>
       </c>
       <c r="N9">
-        <v>0.75</v>
+        <v>-0.3451711635802232</v>
       </c>
       <c r="O9">
-        <v>0.6666666666666666</v>
+        <v>-0.6289483304324449</v>
       </c>
       <c r="P9">
-        <v>0.75</v>
+        <v>-0.3206372558951174</v>
       </c>
       <c r="Q9">
-        <v>0.5</v>
+        <v>-0.08505284855852796</v>
       </c>
       <c r="R9">
-        <v>0.3333333333333333</v>
+        <v>-1.039194290979325</v>
       </c>
       <c r="S9">
-        <v>0.5555555555555555</v>
+        <v>-1.194958832147968</v>
       </c>
       <c r="T9">
-        <v>0.6666666666666666</v>
+        <v>-0.4552089614730434</v>
       </c>
       <c r="U9">
-        <v>0.75</v>
+        <v>-0.4402057576103177</v>
       </c>
       <c r="V9">
-        <v>0.6666666666666666</v>
+        <v>0.03601668464572096</v>
       </c>
       <c r="W9">
-        <v>0.75</v>
+        <v>0.1448158872213257</v>
       </c>
       <c r="X9">
-        <v>0.75</v>
+        <v>-0.2007582490940618</v>
       </c>
       <c r="Y9">
-        <v>0.5</v>
+        <v>-0.2252533884917919</v>
       </c>
       <c r="Z9">
-        <v>0.5</v>
+        <v>-0.4506905521495219</v>
       </c>
       <c r="AA9">
-        <v>0.5</v>
+        <v>-0.4433049424071018</v>
       </c>
       <c r="AB9">
-        <v>0.5</v>
+        <v>-0.1708044864192125</v>
       </c>
       <c r="AC9">
-        <v>0.75</v>
+        <v>0.3651867476594346</v>
       </c>
       <c r="AD9">
-        <v>0.5</v>
+        <v>-0.3675822075682514</v>
       </c>
       <c r="AE9">
-        <v>0.75</v>
+        <v>0.198542512546419</v>
       </c>
       <c r="AF9">
-        <v>0.5</v>
+        <v>-0.8768812412626135</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH9">
-        <v>0.6666666666666666</v>
+        <v>0.9716310621293642</v>
       </c>
       <c r="AI9">
-        <v>1</v>
+        <v>1.753380741118031</v>
       </c>
       <c r="AJ9">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK9">
-        <v>0</v>
+        <v>-0.9282300922017971</v>
       </c>
       <c r="AL9">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM9">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN9">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO9">
-        <v>0</v>
+        <v>-0.32030283871156</v>
       </c>
       <c r="AP9">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ9">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR9">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS9">
-        <v>0</v>
+        <v>-0.4221056548469904</v>
       </c>
       <c r="AT9">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="AU9">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV9">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW9">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX9">
-        <v>1</v>
+        <v>1.503784699035281</v>
       </c>
       <c r="AY9">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ9">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA9">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB9">
-        <v>1</v>
+        <v>0.6860951906939206</v>
       </c>
       <c r="BC9">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD9">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE9">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF9">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG9">
-        <v>0.5</v>
+        <v>0.145181448325954</v>
       </c>
       <c r="BH9">
-        <v>0.25</v>
+        <v>-1.353352309216741</v>
       </c>
       <c r="BI9">
-        <v>0.25</v>
+        <v>0.05207201872289086</v>
       </c>
       <c r="BJ9">
-        <v>1</v>
+        <v>1.549207931076509</v>
       </c>
       <c r="BK9">
-        <v>0.5</v>
+        <v>-0.359884646501022</v>
       </c>
       <c r="BL9">
-        <v>1</v>
+        <v>1.322149158209643</v>
       </c>
       <c r="BM9">
-        <v>0.75</v>
+        <v>0.4605627942900607</v>
       </c>
       <c r="BN9">
-        <v>0.5</v>
+        <v>-0.3053974600325877</v>
       </c>
       <c r="BO9">
-        <v>0.75</v>
+        <v>0.335586194236475</v>
       </c>
       <c r="BP9">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ9">
-        <v>0.5</v>
+        <v>-0.04296330039934874</v>
       </c>
       <c r="BR9">
-        <v>0.25</v>
+        <v>0.3186307268862352</v>
       </c>
       <c r="BS9">
-        <v>0.25</v>
+        <v>-0.3308949948112696</v>
       </c>
       <c r="BT9">
-        <v>1</v>
+        <v>0.9783665806745229</v>
       </c>
       <c r="BU9">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="BV9">
-        <v>0.75</v>
+        <v>0.657827488493832</v>
       </c>
       <c r="BW9">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX9">
-        <v>0.5</v>
+        <v>0.1947373292480012</v>
       </c>
       <c r="BY9">
-        <v>0.75</v>
+        <v>1.440055889940203</v>
       </c>
       <c r="BZ9">
-        <v>0.5</v>
+        <v>1.215702515811881</v>
       </c>
       <c r="CA9">
-        <v>0</v>
+        <v>-0.6319155142804664</v>
       </c>
       <c r="CB9">
-        <v>0.75</v>
+        <v>-0.4962523746607706</v>
       </c>
       <c r="CC9">
-        <v>0.1666666666666667</v>
+        <v>-0.1492371659207503</v>
       </c>
       <c r="CD9">
-        <v>0.6666666666666666</v>
+        <v>0.6048126879380211</v>
       </c>
       <c r="CE9">
-        <v>0.5</v>
+        <v>0.829382348286514</v>
       </c>
       <c r="CF9">
-        <v>1</v>
+        <v>0.9174012913193432</v>
       </c>
       <c r="CG9">
-        <v>0.5</v>
+        <v>-0.07860656409769635</v>
       </c>
     </row>
     <row r="10" spans="1:85">
       <c r="A10">
-        <v>1</v>
+        <v>1.028188860376577</v>
       </c>
       <c r="B10">
-        <v>0.6666666666666666</v>
+        <v>-0.4365385085865857</v>
       </c>
       <c r="C10">
-        <v>0.6666666666666666</v>
+        <v>-0.3617626333365028</v>
       </c>
       <c r="D10">
-        <v>0.6666666666666666</v>
+        <v>-0.2260313209104581</v>
       </c>
       <c r="E10">
-        <v>0.75</v>
+        <v>0.1803145822967834</v>
       </c>
       <c r="F10">
-        <v>0.3333333333333333</v>
+        <v>-1.60286130892507</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>1.393397669927723</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>1.342846313523137</v>
       </c>
       <c r="I10">
-        <v>0.75</v>
+        <v>0.1603933132127148</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0.9806043766748238</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>1.213272816896799</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>-2.554460267673772</v>
       </c>
       <c r="M10">
-        <v>0.8333333333333333</v>
+        <v>0.7310582067081088</v>
       </c>
       <c r="N10">
-        <v>1</v>
+        <v>0.8753825385642784</v>
       </c>
       <c r="O10">
-        <v>1</v>
+        <v>0.745123499747991</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>0.8747820785834173</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>1.304143677897427</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>1.167887082431874</v>
       </c>
       <c r="S10">
-        <v>1</v>
+        <v>1.107686557889971</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>0.8907968470205251</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>0.8180490328925062</v>
       </c>
       <c r="V10">
-        <v>0.7777777777777777</v>
+        <v>0.5731350687101603</v>
       </c>
       <c r="W10">
-        <v>1</v>
+        <v>1.273721553514843</v>
       </c>
       <c r="X10">
-        <v>1</v>
+        <v>1.051243195256178</v>
       </c>
       <c r="Y10">
-        <v>0</v>
+        <v>-2.043180735613784</v>
       </c>
       <c r="Z10">
-        <v>0.25</v>
+        <v>-1.387580609042165</v>
       </c>
       <c r="AA10">
-        <v>0.25</v>
+        <v>-1.387737211013536</v>
       </c>
       <c r="AB10">
-        <v>0.25</v>
+        <v>-1.163786500686837</v>
       </c>
       <c r="AC10">
-        <v>1</v>
+        <v>1.483571162366453</v>
       </c>
       <c r="AD10">
-        <v>1</v>
+        <v>1.904142066231934</v>
       </c>
       <c r="AE10">
-        <v>1</v>
+        <v>1.262606290724883</v>
       </c>
       <c r="AF10">
-        <v>1</v>
+        <v>1.491388567816728</v>
       </c>
       <c r="AG10">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH10">
-        <v>0.6666666666666666</v>
+        <v>0.9716310621293642</v>
       </c>
       <c r="AI10">
-        <v>1</v>
+        <v>1.753380741118031</v>
       </c>
       <c r="AJ10">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK10">
-        <v>0</v>
+        <v>-0.9282300922017971</v>
       </c>
       <c r="AL10">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM10">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN10">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO10">
-        <v>1</v>
+        <v>3.112943213727974</v>
       </c>
       <c r="AP10">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ10">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR10">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS10">
-        <v>0</v>
+        <v>-0.4221056548469904</v>
       </c>
       <c r="AT10">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="AU10">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV10">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW10">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX10">
-        <v>0</v>
+        <v>-1.217349518266656</v>
       </c>
       <c r="AY10">
-        <v>0</v>
+        <v>-1.937244293292677</v>
       </c>
       <c r="AZ10">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA10">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB10">
-        <v>1</v>
+        <v>0.6860951906939206</v>
       </c>
       <c r="BC10">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD10">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE10">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF10">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG10">
-        <v>0</v>
+        <v>-2.01991580279588</v>
       </c>
       <c r="BH10">
-        <v>0</v>
+        <v>-2.035999135777538</v>
       </c>
       <c r="BI10">
-        <v>0</v>
+        <v>-0.8409631023746879</v>
       </c>
       <c r="BJ10">
-        <v>0</v>
+        <v>-2.206115887716724</v>
       </c>
       <c r="BK10">
-        <v>0</v>
+        <v>-1.786941684071548</v>
       </c>
       <c r="BL10">
-        <v>0</v>
+        <v>-2.49677430508221</v>
       </c>
       <c r="BM10">
-        <v>0</v>
+        <v>-1.945117994159039</v>
       </c>
       <c r="BN10">
-        <v>0.5</v>
+        <v>-0.3053974600325877</v>
       </c>
       <c r="BO10">
-        <v>0.5</v>
+        <v>-0.543086054794906</v>
       </c>
       <c r="BP10">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ10">
-        <v>0</v>
+        <v>-2.007818238662891</v>
       </c>
       <c r="BR10">
-        <v>0</v>
+        <v>-0.6400564601486658</v>
       </c>
       <c r="BS10">
-        <v>0</v>
+        <v>-1.171613389035458</v>
       </c>
       <c r="BT10">
-        <v>0</v>
+        <v>-1.019131854869295</v>
       </c>
       <c r="BU10">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="BV10">
-        <v>0</v>
+        <v>-1.55427867379425</v>
       </c>
       <c r="BW10">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX10">
-        <v>0</v>
+        <v>-1.053765547986848</v>
       </c>
       <c r="BY10">
-        <v>0</v>
+        <v>-0.798339141401895</v>
       </c>
       <c r="BZ10">
-        <v>0</v>
+        <v>-0.5109474341818052</v>
       </c>
       <c r="CA10">
-        <v>0</v>
+        <v>-0.6319155142804664</v>
       </c>
       <c r="CB10">
-        <v>0.25</v>
+        <v>-2.87687565450195</v>
       </c>
       <c r="CC10">
-        <v>0.3333333333333333</v>
+        <v>0.4906171829644669</v>
       </c>
       <c r="CD10">
-        <v>1</v>
+        <v>1.59503107439502</v>
       </c>
       <c r="CE10">
-        <v>0</v>
+        <v>-1.173984873278798</v>
       </c>
       <c r="CF10">
-        <v>1</v>
+        <v>0.9174012913193432</v>
       </c>
       <c r="CG10">
-        <v>0.75</v>
+        <v>0.9583954161142225</v>
       </c>
     </row>
     <row r="11" spans="1:85">
       <c r="A11">
-        <v>1</v>
+        <v>1.028188860376577</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>1.154714764648387</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>1.310167374786254</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>1.228245668343623</v>
       </c>
       <c r="E11">
-        <v>0.75</v>
+        <v>0.1803145822967834</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>1.13236968093214</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>1.393397669927723</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>1.342846313523137</v>
       </c>
       <c r="I11">
-        <v>0.75</v>
+        <v>0.1603933132127148</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0.9806043766748238</v>
       </c>
       <c r="K11">
-        <v>0.5</v>
+        <v>-0.8938288347265028</v>
       </c>
       <c r="L11">
-        <v>0.5</v>
+        <v>-0.427810093372549</v>
       </c>
       <c r="M11">
-        <v>0.6666666666666666</v>
+        <v>-0.1160801882273011</v>
       </c>
       <c r="N11">
-        <v>0.75</v>
+        <v>-0.3451711635802232</v>
       </c>
       <c r="O11">
-        <v>0.6666666666666666</v>
+        <v>-0.6289483304324449</v>
       </c>
       <c r="P11">
-        <v>0.75</v>
+        <v>-0.3206372558951174</v>
       </c>
       <c r="Q11">
-        <v>0.5</v>
+        <v>-0.08505284855852796</v>
       </c>
       <c r="R11">
-        <v>0.6666666666666666</v>
+        <v>0.06434639572627425</v>
       </c>
       <c r="S11">
-        <v>0.7777777777777777</v>
+        <v>-0.04363613712899878</v>
       </c>
       <c r="T11">
-        <v>0.6666666666666666</v>
+        <v>-0.4552089614730434</v>
       </c>
       <c r="U11">
-        <v>0.75</v>
+        <v>-0.4402057576103177</v>
       </c>
       <c r="V11">
-        <v>0.6666666666666666</v>
+        <v>0.03601668464572096</v>
       </c>
       <c r="W11">
-        <v>0.75</v>
+        <v>0.1448158872213257</v>
       </c>
       <c r="X11">
-        <v>0.75</v>
+        <v>-0.2007582490940618</v>
       </c>
       <c r="Y11">
-        <v>0.5</v>
+        <v>-0.2252533884917919</v>
       </c>
       <c r="Z11">
-        <v>0.5</v>
+        <v>-0.4506905521495219</v>
       </c>
       <c r="AA11">
-        <v>0.5</v>
+        <v>-0.4433049424071018</v>
       </c>
       <c r="AB11">
-        <v>0.5</v>
+        <v>-0.1708044864192125</v>
       </c>
       <c r="AC11">
-        <v>0.5</v>
+        <v>-0.7531976670475842</v>
       </c>
       <c r="AD11">
-        <v>0.75</v>
+        <v>0.7682799293318415</v>
       </c>
       <c r="AE11">
-        <v>0.75</v>
+        <v>0.198542512546419</v>
       </c>
       <c r="AF11">
-        <v>0.75</v>
+        <v>0.3072536632770573</v>
       </c>
       <c r="AG11">
-        <v>1</v>
+        <v>2.168620633466131</v>
       </c>
       <c r="AH11">
-        <v>0.6666666666666666</v>
+        <v>0.9716310621293642</v>
       </c>
       <c r="AI11">
-        <v>1</v>
+        <v>1.753380741118031</v>
       </c>
       <c r="AJ11">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK11">
-        <v>1</v>
+        <v>1.074178219906482</v>
       </c>
       <c r="AL11">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM11">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN11">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO11">
-        <v>0</v>
+        <v>-0.32030283871156</v>
       </c>
       <c r="AP11">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ11">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR11">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS11">
-        <v>0</v>
+        <v>-0.4221056548469904</v>
       </c>
       <c r="AT11">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="AU11">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV11">
-        <v>1</v>
+        <v>2.505895288430044</v>
       </c>
       <c r="AW11">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX11">
-        <v>1</v>
+        <v>1.503784699035281</v>
       </c>
       <c r="AY11">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ11">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA11">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB11">
-        <v>1</v>
+        <v>0.6860951906939206</v>
       </c>
       <c r="BC11">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD11">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE11">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF11">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG11">
-        <v>0.25</v>
+        <v>-0.937367177234963</v>
       </c>
       <c r="BH11">
-        <v>0.25</v>
+        <v>-1.353352309216741</v>
       </c>
       <c r="BI11">
-        <v>0.25</v>
+        <v>0.05207201872289086</v>
       </c>
       <c r="BJ11">
-        <v>0.25</v>
+        <v>-1.267284933018416</v>
       </c>
       <c r="BK11">
-        <v>0</v>
+        <v>-1.786941684071548</v>
       </c>
       <c r="BL11">
-        <v>0.5</v>
+        <v>-0.5873125734362835</v>
       </c>
       <c r="BM11">
-        <v>0.25</v>
+        <v>-1.143224398009339</v>
       </c>
       <c r="BN11">
-        <v>0.75</v>
+        <v>0.4763288742299319</v>
       </c>
       <c r="BO11">
-        <v>0.5</v>
+        <v>-0.543086054794906</v>
       </c>
       <c r="BP11">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ11">
-        <v>0</v>
+        <v>-2.007818238662891</v>
       </c>
       <c r="BR11">
-        <v>0</v>
+        <v>-0.6400564601486658</v>
       </c>
       <c r="BS11">
-        <v>0.5</v>
+        <v>0.5098233994129192</v>
       </c>
       <c r="BT11">
-        <v>1</v>
+        <v>0.9783665806745229</v>
       </c>
       <c r="BU11">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="BV11">
-        <v>0.75</v>
+        <v>0.657827488493832</v>
       </c>
       <c r="BW11">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX11">
-        <v>0.5</v>
+        <v>0.1947373292480012</v>
       </c>
       <c r="BY11">
-        <v>0</v>
+        <v>-0.798339141401895</v>
       </c>
       <c r="BZ11">
-        <v>0</v>
+        <v>-0.5109474341818052</v>
       </c>
       <c r="CA11">
-        <v>0.25</v>
+        <v>0.3400442229311928</v>
       </c>
       <c r="CB11">
-        <v>0.75</v>
+        <v>-0.4962523746607706</v>
       </c>
       <c r="CC11">
-        <v>0</v>
+        <v>-0.7890915148059675</v>
       </c>
       <c r="CD11">
-        <v>0.6666666666666666</v>
+        <v>0.6048126879380211</v>
       </c>
       <c r="CE11">
-        <v>0.5</v>
+        <v>0.829382348286514</v>
       </c>
       <c r="CF11">
-        <v>1</v>
+        <v>0.9174012913193432</v>
       </c>
       <c r="CG11">
-        <v>0.5</v>
+        <v>-0.07860656409769635</v>
       </c>
     </row>
     <row r="12" spans="1:85">
       <c r="A12">
-        <v>0.6666666666666666</v>
+        <v>-0.3088476044477176</v>
       </c>
       <c r="B12">
-        <v>0.6666666666666666</v>
+        <v>-0.4365385085865857</v>
       </c>
       <c r="C12">
-        <v>0.6666666666666666</v>
+        <v>-0.3617626333365028</v>
       </c>
       <c r="D12">
-        <v>0.6666666666666666</v>
+        <v>-0.2260313209104581</v>
       </c>
       <c r="E12">
-        <v>0.5</v>
+        <v>-0.9616777722495112</v>
       </c>
       <c r="F12">
-        <v>0.3333333333333333</v>
+        <v>-1.60286130892507</v>
       </c>
       <c r="G12">
-        <v>0.5</v>
+        <v>-1.013380123583798</v>
       </c>
       <c r="H12">
-        <v>0.75</v>
+        <v>0.2302948991790885</v>
       </c>
       <c r="I12">
-        <v>0.75</v>
+        <v>0.1603933132127148</v>
       </c>
       <c r="J12">
-        <v>0.25</v>
+        <v>-2.574519617913051</v>
       </c>
       <c r="K12">
-        <v>0.5</v>
+        <v>-0.8938288347265028</v>
       </c>
       <c r="L12">
-        <v>0.75</v>
+        <v>0.6355149937780624</v>
       </c>
       <c r="M12">
-        <v>0.9166666666666667</v>
+        <v>1.154627404175815</v>
       </c>
       <c r="N12">
-        <v>1</v>
+        <v>0.8753825385642784</v>
       </c>
       <c r="O12">
-        <v>1</v>
+        <v>0.745123499747991</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0.8747820785834173</v>
       </c>
       <c r="Q12">
-        <v>0.25</v>
+        <v>-0.7796511117865056</v>
       </c>
       <c r="R12">
-        <v>0.3333333333333333</v>
+        <v>-1.039194290979325</v>
       </c>
       <c r="S12">
-        <v>0.888888888888889</v>
+        <v>0.532025210380487</v>
       </c>
       <c r="T12">
-        <v>1</v>
+        <v>0.8907968470205251</v>
       </c>
       <c r="U12">
-        <v>1</v>
+        <v>0.8180490328925062</v>
       </c>
       <c r="V12">
-        <v>0.7777777777777777</v>
+        <v>0.5731350687101603</v>
       </c>
       <c r="W12">
-        <v>0.5</v>
+        <v>-0.9840897790721913</v>
       </c>
       <c r="X12">
-        <v>1</v>
+        <v>1.051243195256178</v>
       </c>
       <c r="Y12">
-        <v>0.5</v>
+        <v>-0.2252533884917919</v>
       </c>
       <c r="Z12">
-        <v>0.25</v>
+        <v>-1.387580609042165</v>
       </c>
       <c r="AA12">
-        <v>0.75</v>
+        <v>0.5011273261993328</v>
       </c>
       <c r="AB12">
-        <v>0.5</v>
+        <v>-0.1708044864192125</v>
       </c>
       <c r="AC12">
-        <v>0.5</v>
+        <v>-0.7531976670475842</v>
       </c>
       <c r="AD12">
-        <v>0.25</v>
+        <v>-1.503444344468344</v>
       </c>
       <c r="AE12">
-        <v>0.25</v>
+        <v>-1.929585043810508</v>
       </c>
       <c r="AF12">
-        <v>0.25</v>
+        <v>-2.061016145802284</v>
       </c>
       <c r="AG12">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH12">
-        <v>0.3333333333333333</v>
+        <v>-0.04754158102162029</v>
       </c>
       <c r="AI12">
-        <v>0</v>
+        <v>-0.5686640241463884</v>
       </c>
       <c r="AJ12">
-        <v>0</v>
+        <v>-0.3679208923408285</v>
       </c>
       <c r="AK12">
-        <v>0</v>
+        <v>-0.9282300922017971</v>
       </c>
       <c r="AL12">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM12">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN12">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO12">
-        <v>0</v>
+        <v>-0.32030283871156</v>
       </c>
       <c r="AP12">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ12">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR12">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS12">
-        <v>1</v>
+        <v>2.362168183855273</v>
       </c>
       <c r="AT12">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="AU12">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV12">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW12">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="AX12">
-        <v>0.5</v>
+        <v>0.1432175903843125</v>
       </c>
       <c r="AY12">
-        <v>1</v>
+        <v>0.514692210764106</v>
       </c>
       <c r="AZ12">
-        <v>1</v>
+        <v>1.513729497088757</v>
       </c>
       <c r="BA12">
-        <v>0</v>
+        <v>-0.4828367003793034</v>
       </c>
       <c r="BB12">
-        <v>1</v>
+        <v>0.6860951906939206</v>
       </c>
       <c r="BC12">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD12">
-        <v>1</v>
+        <v>2.008065540912678</v>
       </c>
       <c r="BE12">
-        <v>0</v>
+        <v>-1.513729497088757</v>
       </c>
       <c r="BF12">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG12">
-        <v>0.75</v>
+        <v>1.227730073886871</v>
       </c>
       <c r="BH12">
-        <v>1</v>
+        <v>0.6945881704656511</v>
       </c>
       <c r="BI12">
-        <v>0</v>
+        <v>-0.8409631023746879</v>
       </c>
       <c r="BJ12">
-        <v>0.5</v>
+        <v>-0.3284539783201077</v>
       </c>
       <c r="BK12">
-        <v>0.25</v>
+        <v>-1.073413165286285</v>
       </c>
       <c r="BL12">
-        <v>1</v>
+        <v>1.322149158209643</v>
       </c>
       <c r="BM12">
-        <v>0.25</v>
+        <v>-1.143224398009339</v>
       </c>
       <c r="BN12">
-        <v>0.5</v>
+        <v>-0.3053974600325877</v>
       </c>
       <c r="BO12">
-        <v>1</v>
+        <v>1.214258443267856</v>
       </c>
       <c r="BP12">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ12">
-        <v>0</v>
+        <v>-2.007818238662891</v>
       </c>
       <c r="BR12">
-        <v>0</v>
+        <v>-0.6400564601486658</v>
       </c>
       <c r="BS12">
-        <v>0</v>
+        <v>-1.171613389035458</v>
       </c>
       <c r="BT12">
-        <v>1</v>
+        <v>0.9783665806745229</v>
       </c>
       <c r="BU12">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="BV12">
-        <v>1</v>
+        <v>1.395196209256526</v>
       </c>
       <c r="BW12">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX12">
-        <v>0</v>
+        <v>-1.053765547986848</v>
       </c>
       <c r="BY12">
-        <v>0</v>
+        <v>-0.798339141401895</v>
       </c>
       <c r="BZ12">
-        <v>0</v>
+        <v>-0.5109474341818052</v>
       </c>
       <c r="CA12">
-        <v>0</v>
+        <v>-0.6319155142804664</v>
       </c>
       <c r="CB12">
-        <v>1</v>
+        <v>0.6940592652598194</v>
       </c>
       <c r="CC12">
-        <v>0</v>
+        <v>-0.7890915148059675</v>
       </c>
       <c r="CD12">
-        <v>0.5</v>
+        <v>0.1097034947095217</v>
       </c>
       <c r="CE12">
-        <v>0.5</v>
+        <v>0.829382348286514</v>
       </c>
       <c r="CF12">
-        <v>1</v>
+        <v>0.9174012913193432</v>
       </c>
       <c r="CG12">
-        <v>0.75</v>
+        <v>0.9583954161142225</v>
       </c>
     </row>
     <row r="13" spans="1:85">
       <c r="A13">
-        <v>0.6666666666666666</v>
+        <v>-0.3088476044477176</v>
       </c>
       <c r="B13">
-        <v>0.6666666666666666</v>
+        <v>-0.4365385085865857</v>
       </c>
       <c r="C13">
-        <v>0.6666666666666666</v>
+        <v>-0.3617626333365028</v>
       </c>
       <c r="D13">
-        <v>0.6666666666666666</v>
+        <v>-0.2260313209104581</v>
       </c>
       <c r="E13">
-        <v>0.75</v>
+        <v>0.1803145822967834</v>
       </c>
       <c r="F13">
-        <v>0.6666666666666666</v>
+        <v>-0.235245813996465</v>
       </c>
       <c r="G13">
-        <v>0.75</v>
+        <v>0.1900087731719623</v>
       </c>
       <c r="H13">
-        <v>0.75</v>
+        <v>0.2302948991790885</v>
       </c>
       <c r="I13">
-        <v>0.75</v>
+        <v>0.1603933132127148</v>
       </c>
       <c r="J13">
-        <v>0.75</v>
+        <v>-0.2044369548544679</v>
       </c>
       <c r="K13">
-        <v>0.75</v>
+        <v>0.159721991085148</v>
       </c>
       <c r="L13">
-        <v>0.25</v>
+        <v>-1.49113518052316</v>
       </c>
       <c r="M13">
-        <v>0.75</v>
+        <v>0.3074890092404042</v>
       </c>
       <c r="N13">
-        <v>0.75</v>
+        <v>-0.3451711635802232</v>
       </c>
       <c r="O13">
-        <v>0.3333333333333333</v>
+        <v>-2.003020160612881</v>
       </c>
       <c r="P13">
-        <v>0.75</v>
+        <v>-0.3206372558951174</v>
       </c>
       <c r="Q13">
-        <v>0.5</v>
+        <v>-0.08505284855852796</v>
       </c>
       <c r="R13">
-        <v>0.6666666666666666</v>
+        <v>0.06434639572627425</v>
       </c>
       <c r="S13">
-        <v>0.3333333333333333</v>
+        <v>-2.346281527166937</v>
       </c>
       <c r="T13">
-        <v>0.6666666666666666</v>
+        <v>-0.4552089614730434</v>
       </c>
       <c r="U13">
-        <v>0.5</v>
+        <v>-1.698460548113142</v>
       </c>
       <c r="V13">
-        <v>0.6666666666666666</v>
+        <v>0.03601668464572096</v>
       </c>
       <c r="W13">
-        <v>0.75</v>
+        <v>0.1448158872213257</v>
       </c>
       <c r="X13">
-        <v>0.75</v>
+        <v>-0.2007582490940618</v>
       </c>
       <c r="Y13">
-        <v>0.25</v>
+        <v>-1.134217062052788</v>
       </c>
       <c r="Z13">
-        <v>0.25</v>
+        <v>-1.387580609042165</v>
       </c>
       <c r="AA13">
-        <v>0.25</v>
+        <v>-1.387737211013536</v>
       </c>
       <c r="AB13">
-        <v>0.25</v>
+        <v>-1.163786500686837</v>
       </c>
       <c r="AC13">
-        <v>0.5</v>
+        <v>-0.7531976670475842</v>
       </c>
       <c r="AD13">
-        <v>0.5</v>
+        <v>-0.3675822075682514</v>
       </c>
       <c r="AE13">
-        <v>0.75</v>
+        <v>0.198542512546419</v>
       </c>
       <c r="AF13">
-        <v>0.5</v>
+        <v>-0.8768812412626135</v>
       </c>
       <c r="AG13">
-        <v>0</v>
+        <v>-0.4597782261765648</v>
       </c>
       <c r="AH13">
-        <v>0.3333333333333333</v>
+        <v>-0.04754158102162029</v>
       </c>
       <c r="AI13">
-        <v>0</v>
+        <v>-0.5686640241463884</v>
       </c>
       <c r="AJ13">
-        <v>1</v>
+        <v>2.710051450900737</v>
       </c>
       <c r="AK13">
-        <v>0</v>
+        <v>-0.9282300922017971</v>
       </c>
       <c r="AL13">
-        <v>0.3333333333333333</v>
+        <v>-0.1004767233625566</v>
       </c>
       <c r="AM13">
-        <v>0</v>
+        <v>-0.7344512470026582</v>
       </c>
       <c r="AN13">
-        <v>0</v>
+        <v>-0.1901264849878503</v>
       </c>
       <c r="AO13">
-        <v>0</v>
+        <v>-0.32030283871156</v>
       </c>
       <c r="AP13">
-        <v>0</v>
+        <v>-0.1084666281266622</v>
       </c>
       <c r="AQ13">
-        <v>0</v>
+        <v>-0.2059833238555827</v>
       </c>
       <c r="AR13">
-        <v>0</v>
+        <v>-0.1639132322401915</v>
       </c>
       <c r="AS13">
-        <v>0</v>
+        <v>-0.4221056548469904</v>
       </c>
       <c r="AT13">
-        <v>1</v>
+        <v>1.335441221758971</v>
       </c>
       <c r="AU13">
-        <v>0</v>
+        <v>-0.6135221493953239</v>
       </c>
       <c r="AV13">
-        <v>0</v>
+        <v>-0.3978955356628786</v>
       </c>
       <c r="AW13">
-        <v>1</v>
+        <v>2.065055426237636</v>
       </c>
       <c r="AX13">
-        <v>0</v>
+        <v>-1.217349518266656</v>
       </c>
       <c r="AY13">
-        <v>0</v>
+        <v>-1.937244293292677</v>
       </c>
       <c r="AZ13">
-        <v>0</v>
+        <v>-0.6586940071013839</v>
       </c>
       <c r="BA13">
-        <v>1</v>
+        <v>2.065055426237636</v>
       </c>
       <c r="BB13">
-        <v>0</v>
+        <v>-1.45327435846985</v>
       </c>
       <c r="BC13">
-        <v>0</v>
+        <v>-0.3880289404238466</v>
       </c>
       <c r="BD13">
-        <v>0</v>
+        <v>-0.4965398428438622</v>
       </c>
       <c r="BE13">
-        <v>1</v>
+        <v>0.6586940071013839</v>
       </c>
       <c r="BF13">
-        <v>0</v>
+        <v>-0.3312273666228353</v>
       </c>
       <c r="BG13">
-        <v>0.5</v>
+        <v>0.145181448325954</v>
       </c>
       <c r="BH13">
-        <v>0.5</v>
+        <v>-0.6707054826559437</v>
       </c>
       <c r="BI13">
-        <v>0.25</v>
+        <v>0.05207201872289086</v>
       </c>
       <c r="BJ13">
-        <v>0.5</v>
+        <v>-0.3284539783201077</v>
       </c>
       <c r="BK13">
-        <v>1</v>
+        <v>1.067172391069504</v>
       </c>
       <c r="BL13">
-        <v>0.75</v>
+        <v>0.3674182923866799</v>
       </c>
       <c r="BM13">
-        <v>0.5</v>
+        <v>-0.3413308018596391</v>
       </c>
       <c r="BN13">
-        <v>0.75</v>
+        <v>0.4763288742299319</v>
       </c>
       <c r="BO13">
-        <v>0.75</v>
+        <v>0.335586194236475</v>
       </c>
       <c r="BP13">
-        <v>0</v>
+        <v>-0.6130226813318144</v>
       </c>
       <c r="BQ13">
-        <v>0.75</v>
+        <v>0.9394641687324224</v>
       </c>
       <c r="BR13">
-        <v>0.25</v>
+        <v>0.3186307268862352</v>
       </c>
       <c r="BS13">
-        <v>0.5</v>
+        <v>0.5098233994129192</v>
       </c>
       <c r="BT13">
-        <v>0</v>
+        <v>-1.019131854869295</v>
       </c>
       <c r="BU13">
-        <v>0</v>
+        <v>-0.7466330467106973</v>
       </c>
       <c r="BV13">
-        <v>0.5</v>
+        <v>-0.07954123226886212</v>
       </c>
       <c r="BW13">
-        <v>0</v>
+        <v>-0.4885729553642998</v>
       </c>
       <c r="BX13">
-        <v>0.75</v>
+        <v>0.8189887678654258</v>
       </c>
       <c r="BY13">
-        <v>0.75</v>
+        <v>1.440055889940203</v>
       </c>
       <c r="BZ13">
-        <v>0.25</v>
+        <v>0.3523775408150381</v>
       </c>
       <c r="CA13">
-        <v>0.25</v>
+        <v>0.3400442229311928</v>
       </c>
       <c r="CB13">
-        <v>1</v>
+        <v>0.6940592652598194</v>
       </c>
       <c r="CC13">
-        <v>0.3333333333333333</v>
+        <v>0.4906171829644669</v>
       </c>
       <c r="CD13">
-        <v>0.3333333333333333</v>
+        <v>-0.3854056985189777</v>
       </c>
       <c r="CE13">
-        <v>0</v>
+        <v>-1.173984873278798</v>
       </c>
       <c r="CF13">
-        <v>1</v>
+        <v>0.9174012913193432</v>
       </c>
       <c r="CG13">
-        <v>0.25</v>
+        <v>-1.115608544309615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update normalization in the preprocessing file such that only ordinal (non binary) columns are z-scored.
</commit_message>
<xml_diff>
--- a/items_maps/dropped_lines.xlsx
+++ b/items_maps/dropped_lines.xlsx
@@ -987,19 +987,19 @@
         <v>-0.8768812412626135</v>
       </c>
       <c r="AG2">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH2">
         <v>-1.066714224172605</v>
       </c>
       <c r="AI2">
-        <v>-0.5686640241463884</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>1.074178219906482</v>
+        <v>1</v>
       </c>
       <c r="AL2">
         <v>-0.1004767233625566</v>
@@ -1008,61 +1008,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN2">
-        <v>5.244322210914872</v>
+        <v>1</v>
       </c>
       <c r="AO2">
-        <v>3.112943213727974</v>
+        <v>1</v>
       </c>
       <c r="AP2">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ2">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR2">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS2">
-        <v>2.362168183855273</v>
+        <v>1</v>
       </c>
       <c r="AT2">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="AU2">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV2">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW2">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX2">
         <v>0.1432175903843125</v>
       </c>
       <c r="AY2">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ2">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA2">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB2">
-        <v>0.6860951906939206</v>
+        <v>1</v>
       </c>
       <c r="BC2">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD2">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE2">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF2">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG2">
         <v>-0.937367177234963</v>
@@ -1104,10 +1104,10 @@
         <v>2.191260187861297</v>
       </c>
       <c r="BT2">
-        <v>0.9783665806745229</v>
+        <v>1</v>
       </c>
       <c r="BU2">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="BV2">
         <v>0.657827488493832</v>
@@ -1140,7 +1140,7 @@
         <v>0.829382348286514</v>
       </c>
       <c r="CF2">
-        <v>-1.086857580798712</v>
+        <v>0</v>
       </c>
       <c r="CG2">
         <v>-0.07860656409769635</v>
@@ -1244,19 +1244,19 @@
         <v>-0.8768812412626135</v>
       </c>
       <c r="AG3">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH3">
         <v>-1.066714224172605</v>
       </c>
       <c r="AI3">
-        <v>-0.5686640241463884</v>
+        <v>0</v>
       </c>
       <c r="AJ3">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK3">
-        <v>1.074178219906482</v>
+        <v>1</v>
       </c>
       <c r="AL3">
         <v>-0.1004767233625566</v>
@@ -1265,61 +1265,61 @@
         <v>0.7474121513615285</v>
       </c>
       <c r="AN3">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO3">
-        <v>3.112943213727974</v>
+        <v>1</v>
       </c>
       <c r="AP3">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ3">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR3">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS3">
-        <v>-0.4221056548469904</v>
+        <v>0</v>
       </c>
       <c r="AT3">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="AU3">
-        <v>1.625181012759954</v>
+        <v>1</v>
       </c>
       <c r="AV3">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW3">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX3">
         <v>0.1432175903843125</v>
       </c>
       <c r="AY3">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ3">
-        <v>1.513729497088757</v>
+        <v>1</v>
       </c>
       <c r="BA3">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB3">
-        <v>-1.45327435846985</v>
+        <v>0</v>
       </c>
       <c r="BC3">
-        <v>2.56961387214014</v>
+        <v>1</v>
       </c>
       <c r="BD3">
-        <v>2.008065540912678</v>
+        <v>1</v>
       </c>
       <c r="BE3">
-        <v>-1.513729497088757</v>
+        <v>0</v>
       </c>
       <c r="BF3">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG3">
         <v>1.227730073886871</v>
@@ -1361,10 +1361,10 @@
         <v>0.5098233994129192</v>
       </c>
       <c r="BT3">
-        <v>0.9783665806745229</v>
+        <v>1</v>
       </c>
       <c r="BU3">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="BV3">
         <v>0.657827488493832</v>
@@ -1397,7 +1397,7 @@
         <v>0.829382348286514</v>
       </c>
       <c r="CF3">
-        <v>-1.086857580798712</v>
+        <v>0</v>
       </c>
       <c r="CG3">
         <v>-0.07860656409769635</v>
@@ -1501,19 +1501,19 @@
         <v>-0.8768812412626135</v>
       </c>
       <c r="AG4">
-        <v>2.168620633466131</v>
+        <v>1</v>
       </c>
       <c r="AH4">
         <v>-0.04754158102162029</v>
       </c>
       <c r="AI4">
-        <v>-0.5686640241463884</v>
+        <v>0</v>
       </c>
       <c r="AJ4">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK4">
-        <v>1.074178219906482</v>
+        <v>1</v>
       </c>
       <c r="AL4">
         <v>-0.1004767233625566</v>
@@ -1522,61 +1522,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN4">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO4">
-        <v>-0.32030283871156</v>
+        <v>0</v>
       </c>
       <c r="AP4">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ4">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR4">
-        <v>6.083002174247108</v>
+        <v>1</v>
       </c>
       <c r="AS4">
-        <v>-0.4221056548469904</v>
+        <v>0</v>
       </c>
       <c r="AT4">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="AU4">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV4">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW4">
-        <v>2.065055426237636</v>
+        <v>1</v>
       </c>
       <c r="AX4">
         <v>-1.217349518266656</v>
       </c>
       <c r="AY4">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ4">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA4">
-        <v>2.065055426237636</v>
+        <v>1</v>
       </c>
       <c r="BB4">
-        <v>-1.45327435846985</v>
+        <v>0</v>
       </c>
       <c r="BC4">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD4">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE4">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF4">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG4">
         <v>0.145181448325954</v>
@@ -1618,10 +1618,10 @@
         <v>-1.171613389035458</v>
       </c>
       <c r="BT4">
-        <v>0.9783665806745229</v>
+        <v>1</v>
       </c>
       <c r="BU4">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="BV4">
         <v>-1.55427867379425</v>
@@ -1654,7 +1654,7 @@
         <v>0.829382348286514</v>
       </c>
       <c r="CF4">
-        <v>0.9174012913193432</v>
+        <v>1</v>
       </c>
       <c r="CG4">
         <v>-0.07860656409769635</v>
@@ -1758,19 +1758,19 @@
         <v>1.491388567816728</v>
       </c>
       <c r="AG5">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH5">
         <v>-1.066714224172605</v>
       </c>
       <c r="AI5">
-        <v>-0.5686640241463884</v>
+        <v>0</v>
       </c>
       <c r="AJ5">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK5">
-        <v>-0.9282300922017971</v>
+        <v>0</v>
       </c>
       <c r="AL5">
         <v>-0.1004767233625566</v>
@@ -1779,61 +1779,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN5">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO5">
-        <v>-0.32030283871156</v>
+        <v>0</v>
       </c>
       <c r="AP5">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ5">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR5">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS5">
-        <v>2.362168183855273</v>
+        <v>1</v>
       </c>
       <c r="AT5">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="AU5">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV5">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW5">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX5">
         <v>-1.217349518266656</v>
       </c>
       <c r="AY5">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ5">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA5">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB5">
-        <v>-1.45327435846985</v>
+        <v>0</v>
       </c>
       <c r="BC5">
-        <v>2.56961387214014</v>
+        <v>1</v>
       </c>
       <c r="BD5">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE5">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF5">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG5">
         <v>-0.937367177234963</v>
@@ -1875,10 +1875,10 @@
         <v>0.5098233994129192</v>
       </c>
       <c r="BT5">
-        <v>0.9783665806745229</v>
+        <v>1</v>
       </c>
       <c r="BU5">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="BV5">
         <v>-0.07954123226886212</v>
@@ -1911,7 +1911,7 @@
         <v>-1.173984873278798</v>
       </c>
       <c r="CF5">
-        <v>-1.086857580798712</v>
+        <v>0</v>
       </c>
       <c r="CG5">
         <v>-1.115608544309615</v>
@@ -2012,19 +2012,19 @@
         <v>0.3072536632770573</v>
       </c>
       <c r="AG6">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH6">
         <v>0.9716310621293642</v>
       </c>
       <c r="AI6">
-        <v>1.753380741118031</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK6">
-        <v>-0.9282300922017971</v>
+        <v>0</v>
       </c>
       <c r="AL6">
         <v>1.713392545761488</v>
@@ -2033,61 +2033,61 @@
         <v>0.7474121513615285</v>
       </c>
       <c r="AN6">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO6">
-        <v>-0.32030283871156</v>
+        <v>0</v>
       </c>
       <c r="AP6">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ6">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR6">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS6">
-        <v>-0.4221056548469904</v>
+        <v>0</v>
       </c>
       <c r="AT6">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="AU6">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV6">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW6">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX6">
         <v>0.1432175903843125</v>
       </c>
       <c r="AY6">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ6">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA6">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB6">
-        <v>0.6860951906939206</v>
+        <v>1</v>
       </c>
       <c r="BC6">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD6">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE6">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF6">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG6">
         <v>-0.937367177234963</v>
@@ -2129,10 +2129,10 @@
         <v>0.5098233994129192</v>
       </c>
       <c r="BT6">
-        <v>0.9783665806745229</v>
+        <v>1</v>
       </c>
       <c r="BU6">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="BV6">
         <v>-1.55427867379425</v>
@@ -2165,7 +2165,7 @@
         <v>0.829382348286514</v>
       </c>
       <c r="CF6">
-        <v>0.9174012913193432</v>
+        <v>1</v>
       </c>
       <c r="CG6">
         <v>1.995397396326141</v>
@@ -2269,19 +2269,19 @@
         <v>-0.8768812412626135</v>
       </c>
       <c r="AG7">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH7">
         <v>-0.04754158102162029</v>
       </c>
       <c r="AI7">
-        <v>1.753380741118031</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK7">
-        <v>-0.9282300922017971</v>
+        <v>0</v>
       </c>
       <c r="AL7">
         <v>-0.1004767233625566</v>
@@ -2290,61 +2290,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN7">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO7">
-        <v>-0.32030283871156</v>
+        <v>0</v>
       </c>
       <c r="AP7">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ7">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR7">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS7">
-        <v>-0.4221056548469904</v>
+        <v>0</v>
       </c>
       <c r="AT7">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="AU7">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV7">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW7">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX7">
         <v>-1.217349518266656</v>
       </c>
       <c r="AY7">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ7">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA7">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB7">
-        <v>0.6860951906939206</v>
+        <v>1</v>
       </c>
       <c r="BC7">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD7">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE7">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF7">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG7">
         <v>1.227730073886871</v>
@@ -2386,10 +2386,10 @@
         <v>1.350541793637108</v>
       </c>
       <c r="BT7">
-        <v>-1.019131854869295</v>
+        <v>0</v>
       </c>
       <c r="BU7">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="BV7">
         <v>0.657827488493832</v>
@@ -2422,7 +2422,7 @@
         <v>0.829382348286514</v>
       </c>
       <c r="CF7">
-        <v>0.9174012913193432</v>
+        <v>1</v>
       </c>
       <c r="CG7">
         <v>0.9583954161142225</v>
@@ -2526,19 +2526,19 @@
         <v>-0.8768812412626135</v>
       </c>
       <c r="AG8">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH8">
         <v>0.9716310621293642</v>
       </c>
       <c r="AI8">
-        <v>-0.5686640241463884</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK8">
-        <v>-0.9282300922017971</v>
+        <v>0</v>
       </c>
       <c r="AL8">
         <v>-0.1004767233625566</v>
@@ -2547,61 +2547,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN8">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO8">
-        <v>-0.32030283871156</v>
+        <v>0</v>
       </c>
       <c r="AP8">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ8">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR8">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS8">
-        <v>2.362168183855273</v>
+        <v>1</v>
       </c>
       <c r="AT8">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="AU8">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV8">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW8">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX8">
         <v>1.503784699035281</v>
       </c>
       <c r="AY8">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ8">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA8">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB8">
-        <v>0.6860951906939206</v>
+        <v>1</v>
       </c>
       <c r="BC8">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD8">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE8">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF8">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG8">
         <v>-0.937367177234963</v>
@@ -2643,10 +2643,10 @@
         <v>1.350541793637108</v>
       </c>
       <c r="BT8">
-        <v>0.9783665806745229</v>
+        <v>1</v>
       </c>
       <c r="BU8">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="BV8">
         <v>0.657827488493832</v>
@@ -2679,7 +2679,7 @@
         <v>0.829382348286514</v>
       </c>
       <c r="CF8">
-        <v>0.9174012913193432</v>
+        <v>1</v>
       </c>
       <c r="CG8">
         <v>-0.07860656409769635</v>
@@ -2783,19 +2783,19 @@
         <v>-0.8768812412626135</v>
       </c>
       <c r="AG9">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH9">
         <v>0.9716310621293642</v>
       </c>
       <c r="AI9">
-        <v>1.753380741118031</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK9">
-        <v>-0.9282300922017971</v>
+        <v>0</v>
       </c>
       <c r="AL9">
         <v>-0.1004767233625566</v>
@@ -2804,61 +2804,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN9">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO9">
-        <v>-0.32030283871156</v>
+        <v>0</v>
       </c>
       <c r="AP9">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ9">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR9">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS9">
-        <v>-0.4221056548469904</v>
+        <v>0</v>
       </c>
       <c r="AT9">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="AU9">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV9">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW9">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX9">
         <v>1.503784699035281</v>
       </c>
       <c r="AY9">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ9">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA9">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB9">
-        <v>0.6860951906939206</v>
+        <v>1</v>
       </c>
       <c r="BC9">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD9">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE9">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF9">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG9">
         <v>0.145181448325954</v>
@@ -2900,10 +2900,10 @@
         <v>-0.3308949948112696</v>
       </c>
       <c r="BT9">
-        <v>0.9783665806745229</v>
+        <v>1</v>
       </c>
       <c r="BU9">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="BV9">
         <v>0.657827488493832</v>
@@ -2936,7 +2936,7 @@
         <v>0.829382348286514</v>
       </c>
       <c r="CF9">
-        <v>0.9174012913193432</v>
+        <v>1</v>
       </c>
       <c r="CG9">
         <v>-0.07860656409769635</v>
@@ -3040,19 +3040,19 @@
         <v>1.491388567816728</v>
       </c>
       <c r="AG10">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH10">
         <v>0.9716310621293642</v>
       </c>
       <c r="AI10">
-        <v>1.753380741118031</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK10">
-        <v>-0.9282300922017971</v>
+        <v>0</v>
       </c>
       <c r="AL10">
         <v>-0.1004767233625566</v>
@@ -3061,61 +3061,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN10">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO10">
-        <v>3.112943213727974</v>
+        <v>1</v>
       </c>
       <c r="AP10">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ10">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR10">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS10">
-        <v>-0.4221056548469904</v>
+        <v>0</v>
       </c>
       <c r="AT10">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="AU10">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV10">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW10">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX10">
         <v>-1.217349518266656</v>
       </c>
       <c r="AY10">
-        <v>-1.937244293292677</v>
+        <v>0</v>
       </c>
       <c r="AZ10">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA10">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB10">
-        <v>0.6860951906939206</v>
+        <v>1</v>
       </c>
       <c r="BC10">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD10">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE10">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF10">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG10">
         <v>-2.01991580279588</v>
@@ -3157,10 +3157,10 @@
         <v>-1.171613389035458</v>
       </c>
       <c r="BT10">
-        <v>-1.019131854869295</v>
+        <v>0</v>
       </c>
       <c r="BU10">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="BV10">
         <v>-1.55427867379425</v>
@@ -3193,7 +3193,7 @@
         <v>-1.173984873278798</v>
       </c>
       <c r="CF10">
-        <v>0.9174012913193432</v>
+        <v>1</v>
       </c>
       <c r="CG10">
         <v>0.9583954161142225</v>
@@ -3297,19 +3297,19 @@
         <v>0.3072536632770573</v>
       </c>
       <c r="AG11">
-        <v>2.168620633466131</v>
+        <v>1</v>
       </c>
       <c r="AH11">
         <v>0.9716310621293642</v>
       </c>
       <c r="AI11">
-        <v>1.753380741118031</v>
+        <v>1</v>
       </c>
       <c r="AJ11">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK11">
-        <v>1.074178219906482</v>
+        <v>1</v>
       </c>
       <c r="AL11">
         <v>-0.1004767233625566</v>
@@ -3318,61 +3318,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN11">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO11">
-        <v>-0.32030283871156</v>
+        <v>0</v>
       </c>
       <c r="AP11">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ11">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR11">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS11">
-        <v>-0.4221056548469904</v>
+        <v>0</v>
       </c>
       <c r="AT11">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="AU11">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV11">
-        <v>2.505895288430044</v>
+        <v>1</v>
       </c>
       <c r="AW11">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX11">
         <v>1.503784699035281</v>
       </c>
       <c r="AY11">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ11">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA11">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB11">
-        <v>0.6860951906939206</v>
+        <v>1</v>
       </c>
       <c r="BC11">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD11">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE11">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF11">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG11">
         <v>-0.937367177234963</v>
@@ -3414,10 +3414,10 @@
         <v>0.5098233994129192</v>
       </c>
       <c r="BT11">
-        <v>0.9783665806745229</v>
+        <v>1</v>
       </c>
       <c r="BU11">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="BV11">
         <v>0.657827488493832</v>
@@ -3450,7 +3450,7 @@
         <v>0.829382348286514</v>
       </c>
       <c r="CF11">
-        <v>0.9174012913193432</v>
+        <v>1</v>
       </c>
       <c r="CG11">
         <v>-0.07860656409769635</v>
@@ -3554,19 +3554,19 @@
         <v>-2.061016145802284</v>
       </c>
       <c r="AG12">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH12">
         <v>-0.04754158102162029</v>
       </c>
       <c r="AI12">
-        <v>-0.5686640241463884</v>
+        <v>0</v>
       </c>
       <c r="AJ12">
-        <v>-0.3679208923408285</v>
+        <v>0</v>
       </c>
       <c r="AK12">
-        <v>-0.9282300922017971</v>
+        <v>0</v>
       </c>
       <c r="AL12">
         <v>-0.1004767233625566</v>
@@ -3575,61 +3575,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN12">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO12">
-        <v>-0.32030283871156</v>
+        <v>0</v>
       </c>
       <c r="AP12">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ12">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR12">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS12">
-        <v>2.362168183855273</v>
+        <v>1</v>
       </c>
       <c r="AT12">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="AU12">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV12">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW12">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="AX12">
         <v>0.1432175903843125</v>
       </c>
       <c r="AY12">
-        <v>0.514692210764106</v>
+        <v>1</v>
       </c>
       <c r="AZ12">
-        <v>1.513729497088757</v>
+        <v>1</v>
       </c>
       <c r="BA12">
-        <v>-0.4828367003793034</v>
+        <v>0</v>
       </c>
       <c r="BB12">
-        <v>0.6860951906939206</v>
+        <v>1</v>
       </c>
       <c r="BC12">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD12">
-        <v>2.008065540912678</v>
+        <v>1</v>
       </c>
       <c r="BE12">
-        <v>-1.513729497088757</v>
+        <v>0</v>
       </c>
       <c r="BF12">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG12">
         <v>1.227730073886871</v>
@@ -3671,10 +3671,10 @@
         <v>-1.171613389035458</v>
       </c>
       <c r="BT12">
-        <v>0.9783665806745229</v>
+        <v>1</v>
       </c>
       <c r="BU12">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="BV12">
         <v>1.395196209256526</v>
@@ -3707,7 +3707,7 @@
         <v>0.829382348286514</v>
       </c>
       <c r="CF12">
-        <v>0.9174012913193432</v>
+        <v>1</v>
       </c>
       <c r="CG12">
         <v>0.9583954161142225</v>
@@ -3811,19 +3811,19 @@
         <v>-0.8768812412626135</v>
       </c>
       <c r="AG13">
-        <v>-0.4597782261765648</v>
+        <v>0</v>
       </c>
       <c r="AH13">
         <v>-0.04754158102162029</v>
       </c>
       <c r="AI13">
-        <v>-0.5686640241463884</v>
+        <v>0</v>
       </c>
       <c r="AJ13">
-        <v>2.710051450900737</v>
+        <v>1</v>
       </c>
       <c r="AK13">
-        <v>-0.9282300922017971</v>
+        <v>0</v>
       </c>
       <c r="AL13">
         <v>-0.1004767233625566</v>
@@ -3832,61 +3832,61 @@
         <v>-0.7344512470026582</v>
       </c>
       <c r="AN13">
-        <v>-0.1901264849878503</v>
+        <v>0</v>
       </c>
       <c r="AO13">
-        <v>-0.32030283871156</v>
+        <v>0</v>
       </c>
       <c r="AP13">
-        <v>-0.1084666281266622</v>
+        <v>0</v>
       </c>
       <c r="AQ13">
-        <v>-0.2059833238555827</v>
+        <v>0</v>
       </c>
       <c r="AR13">
-        <v>-0.1639132322401915</v>
+        <v>0</v>
       </c>
       <c r="AS13">
-        <v>-0.4221056548469904</v>
+        <v>0</v>
       </c>
       <c r="AT13">
-        <v>1.335441221758971</v>
+        <v>1</v>
       </c>
       <c r="AU13">
-        <v>-0.6135221493953239</v>
+        <v>0</v>
       </c>
       <c r="AV13">
-        <v>-0.3978955356628786</v>
+        <v>0</v>
       </c>
       <c r="AW13">
-        <v>2.065055426237636</v>
+        <v>1</v>
       </c>
       <c r="AX13">
         <v>-1.217349518266656</v>
       </c>
       <c r="AY13">
-        <v>-1.937244293292677</v>
+        <v>0</v>
       </c>
       <c r="AZ13">
-        <v>-0.6586940071013839</v>
+        <v>0</v>
       </c>
       <c r="BA13">
-        <v>2.065055426237636</v>
+        <v>1</v>
       </c>
       <c r="BB13">
-        <v>-1.45327435846985</v>
+        <v>0</v>
       </c>
       <c r="BC13">
-        <v>-0.3880289404238466</v>
+        <v>0</v>
       </c>
       <c r="BD13">
-        <v>-0.4965398428438622</v>
+        <v>0</v>
       </c>
       <c r="BE13">
-        <v>0.6586940071013839</v>
+        <v>1</v>
       </c>
       <c r="BF13">
-        <v>-0.3312273666228353</v>
+        <v>0</v>
       </c>
       <c r="BG13">
         <v>0.145181448325954</v>
@@ -3928,10 +3928,10 @@
         <v>0.5098233994129192</v>
       </c>
       <c r="BT13">
-        <v>-1.019131854869295</v>
+        <v>0</v>
       </c>
       <c r="BU13">
-        <v>-0.7466330467106973</v>
+        <v>0</v>
       </c>
       <c r="BV13">
         <v>-0.07954123226886212</v>
@@ -3964,7 +3964,7 @@
         <v>-1.173984873278798</v>
       </c>
       <c r="CF13">
-        <v>0.9174012913193432</v>
+        <v>1</v>
       </c>
       <c r="CG13">
         <v>-1.115608544309615</v>

</xml_diff>